<commit_message>
test #7 befor update
</commit_message>
<xml_diff>
--- a/gesture_data.xlsx
+++ b/gesture_data.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-1185" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gestures Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:B280"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -434,1754 +433,2792 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[174, 443], [232, 426], [281, 392], [315, 359], [344, 339], [247, 308], [272, 259], [285, 228], [294, 200], [212, 297], [220, 237], [224, 199], [224, 167], [178, 302], [173, 244], [170, 206], [168, 173], [146, 319], [124, 277], [112, 248], [103, 220]]</t>
+          <t>[[287, 274], [326, 259], [355, 235], [367, 206], [353, 191], [336, 210], [342, 187], [341, 210], [339, 220], [316, 207], [323, 183], [322, 211], [317, 221], [295, 206], [303, 183], [304, 212], [300, 223], [271, 207], [281, 189], [285, 209], [283, 220]]</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A3" t="n">
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[[177, 445], [234, 428], [282, 393], [316, 360], [345, 340], [248, 310], [273, 261], [286, 230], [295, 201], [213, 299], [220, 239], [224, 201], [225, 169], [179, 304], [173, 247], [170, 208], [168, 174], [146, 321], [124, 280], [112, 251], [103, 222]]</t>
+          <t>[[298, 274], [338, 258], [364, 234], [376, 206], [363, 193], [344, 209], [351, 187], [351, 210], [347, 221], [324, 206], [333, 183], [332, 212], [326, 221], [304, 206], [314, 183], [315, 212], [309, 223], [281, 207], [292, 189], [297, 208], [294, 219]]</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A4" t="n">
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[[186, 441], [242, 423], [289, 388], [321, 356], [349, 335], [251, 307], [276, 258], [290, 227], [300, 198], [217, 297], [225, 237], [228, 198], [230, 165], [184, 302], [177, 244], [174, 205], [172, 170], [151, 319], [127, 278], [112, 249], [102, 220]]</t>
+          <t>[[302, 273], [342, 258], [369, 234], [380, 206], [366, 192], [346, 208], [355, 187], [355, 210], [350, 222], [328, 205], [338, 183], [337, 212], [330, 223], [308, 205], [319, 183], [320, 213], [313, 224], [285, 206], [298, 188], [302, 208], [299, 220]]</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A5" t="n">
+        <v>0</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[[188, 434], [244, 415], [291, 381], [321, 349], [349, 328], [253, 302], [278, 253], [291, 221], [301, 193], [218, 292], [226, 232], [230, 193], [231, 160], [185, 297], [179, 239], [176, 200], [175, 165], [152, 314], [128, 273], [114, 244], [104, 215]]</t>
+          <t>[[304, 270], [343, 257], [370, 233], [382, 206], [370, 192], [348, 207], [356, 184], [357, 207], [353, 220], [330, 205], [339, 181], [338, 210], [332, 221], [310, 204], [320, 182], [322, 210], [316, 223], [286, 206], [299, 187], [304, 207], [301, 219]]</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A6" t="n">
+        <v>0</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[[188, 441], [244, 423], [290, 387], [322, 353], [350, 332], [254, 305], [279, 255], [292, 224], [301, 195], [220, 296], [227, 236], [231, 197], [231, 163], [186, 301], [181, 243], [178, 204], [176, 169], [153, 319], [130, 278], [116, 249], [106, 220]]</t>
+          <t>[[304, 269], [343, 256], [371, 233], [382, 205], [370, 191], [350, 206], [357, 184], [357, 207], [354, 220], [331, 204], [339, 180], [339, 209], [333, 221], [310, 204], [321, 181], [322, 210], [317, 223], [287, 205], [300, 187], [304, 207], [301, 218]]</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A7" t="n">
+        <v>0</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[[506, 368], [551, 364], [584, 339], [605, 316], [623, 304], [560, 262], [579, 229], [589, 208], [593, 190], [535, 249], [542, 199], [546, 171], [546, 150], [512, 248], [506, 198], [503, 167], [498, 141], [490, 257], [476, 217], [468, 190], [461, 168]]</t>
+          <t>[[306, 271], [347, 259], [374, 234], [384, 206], [372, 192], [351, 208], [359, 185], [360, 208], [356, 221], [332, 206], [342, 182], [342, 211], [335, 222], [312, 205], [324, 183], [325, 212], [318, 224], [289, 207], [303, 188], [307, 208], [302, 219]]</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A8" t="n">
+        <v>0</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[[516, 368], [562, 362], [592, 334], [615, 310], [636, 301], [566, 260], [585, 226], [594, 205], [598, 186], [543, 247], [551, 196], [555, 168], [555, 146], [521, 247], [517, 197], [514, 166], [507, 139], [499, 257], [488, 217], [480, 191], [472, 167]]</t>
+          <t>[[308, 274], [348, 262], [376, 239], [388, 211], [375, 197], [355, 212], [364, 192], [363, 215], [359, 226], [336, 209], [346, 187], [345, 215], [338, 225], [316, 209], [327, 187], [328, 216], [322, 227], [292, 210], [306, 192], [309, 212], [305, 223]]</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A9" t="n">
+        <v>0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[[458, 359], [509, 350], [542, 321], [565, 295], [585, 284], [511, 248], [530, 211], [539, 187], [542, 166], [485, 235], [493, 184], [496, 153], [494, 129], [460, 235], [455, 186], [450, 155], [444, 127], [436, 246], [420, 207], [410, 182], [400, 158]]</t>
+          <t>[[277, 347], [311, 331], [342, 310], [349, 284], [335, 269], [324, 281], [333, 264], [331, 287], [327, 295], [305, 278], [312, 264], [311, 288], [307, 296], [285, 279], [291, 266], [294, 289], [291, 297], [264, 282], [272, 272], [277, 287], [276, 295]]</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A10" t="n">
+        <v>0</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[[458, 365], [509, 357], [543, 328], [565, 303], [586, 290], [512, 254], [532, 216], [541, 192], [546, 170], [486, 241], [493, 189], [497, 158], [497, 134], [460, 242], [455, 192], [452, 160], [448, 132], [437, 253], [420, 213], [409, 188], [400, 164]]</t>
+          <t>[[292, 275], [333, 258], [364, 241], [378, 217], [370, 202], [352, 216], [362, 199], [359, 217], [357, 221], [336, 210], [348, 192], [343, 217], [339, 221], [320, 207], [330, 191], [326, 216], [322, 221], [300, 205], [310, 193], [309, 211], [306, 217]]</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A11" t="n">
+        <v>0</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[[313, 415], [283, 389], [262, 358], [245, 330], [227, 315], [302, 323], [293, 279], [288, 256], [286, 237], [326, 324], [332, 280], [338, 256], [342, 241], [346, 334], [364, 298], [375, 277], [382, 261], [361, 348], [380, 324], [388, 313], [394, 304]]</t>
+          <t>[[292, 243], [328, 237], [359, 223], [373, 200], [363, 185], [349, 201], [357, 183], [354, 192], [350, 199], [333, 193], [342, 174], [334, 196], [331, 206], [316, 188], [324, 171], [318, 194], [314, 205], [295, 186], [304, 173], [304, 189], [301, 198]]</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A12" t="n">
+        <v>0</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[[315, 415], [285, 389], [266, 359], [250, 331], [232, 317], [306, 326], [298, 283], [294, 259], [292, 240], [329, 327], [337, 284], [343, 261], [348, 247], [349, 337], [367, 302], [379, 281], [386, 267], [364, 350], [384, 329], [392, 319], [399, 311]]</t>
+          <t>[[291, 241], [325, 240], [356, 225], [370, 201], [361, 187], [346, 201], [355, 183], [349, 200], [346, 208], [329, 194], [338, 177], [331, 201], [328, 206], [312, 190], [321, 174], [315, 199], [312, 206], [292, 186], [300, 175], [299, 193], [297, 200]]</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A13" t="n">
+        <v>0</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[[316, 416], [287, 390], [268, 359], [253, 331], [235, 316], [309, 326], [302, 283], [298, 260], [297, 241], [333, 328], [341, 285], [348, 264], [353, 250], [352, 338], [369, 303], [381, 283], [388, 268], [367, 352], [386, 332], [396, 322], [403, 313]]</t>
+          <t>[[246, 207], [276, 204], [305, 189], [317, 168], [311, 156], [305, 171], [312, 154], [301, 166], [296, 178], [292, 166], [292, 149], [282, 167], [281, 177], [278, 163], [277, 148], [269, 166], [269, 176], [263, 160], [264, 149], [258, 163], [257, 173]]</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A14" t="n">
+        <v>0</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[[320, 416], [290, 390], [271, 359], [255, 331], [238, 316], [312, 325], [304, 284], [301, 260], [299, 241], [335, 328], [343, 287], [349, 265], [355, 250], [354, 338], [371, 304], [382, 284], [390, 269], [369, 353], [388, 332], [397, 322], [404, 313]]</t>
+          <t>[[192, 209], [217, 203], [241, 188], [246, 164], [239, 153], [244, 177], [245, 153], [234, 165], [233, 176], [229, 172], [227, 151], [218, 170], [220, 179], [216, 169], [211, 153], [204, 173], [207, 181], [202, 167], [198, 156], [194, 171], [196, 179]]</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A15" t="n">
+        <v>0</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[[320, 417], [291, 390], [273, 359], [257, 330], [240, 315], [315, 326], [307, 284], [304, 260], [303, 241], [338, 328], [346, 287], [353, 266], [358, 252], [357, 339], [373, 305], [385, 285], [393, 269], [370, 355], [390, 335], [400, 323], [408, 314]]</t>
+          <t>[[180, 225], [204, 217], [226, 201], [229, 177], [218, 167], [231, 192], [228, 169], [219, 181], [219, 190], [215, 188], [211, 166], [203, 187], [207, 193], [200, 185], [195, 168], [189, 189], [194, 196], [186, 183], [182, 171], [179, 186], [182, 193]]</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A16" t="n">
+        <v>0</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[[271, 452], [314, 437], [351, 408], [376, 383], [396, 368], [319, 346], [341, 312], [353, 291], [361, 273], [292, 339], [297, 293], [299, 265], [298, 243], [267, 343], [259, 301], [253, 274], [247, 251], [244, 356], [227, 326], [216, 306], [207, 287]]</t>
+          <t>[[187, 229], [214, 221], [238, 206], [241, 181], [229, 170], [240, 195], [240, 173], [231, 188], [231, 196], [225, 190], [222, 170], [215, 192], [219, 197], [210, 186], [204, 171], [200, 193], [205, 199], [195, 184], [191, 173], [188, 188], [190, 194]]</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A17" t="n">
+        <v>0</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[[277, 447], [320, 432], [356, 405], [380, 379], [399, 363], [324, 343], [345, 309], [357, 288], [364, 269], [297, 335], [301, 289], [304, 262], [303, 240], [272, 339], [263, 298], [258, 271], [252, 248], [249, 353], [232, 323], [222, 303], [213, 284]]</t>
+          <t>[[246, 266], [295, 257], [347, 218], [363, 171], [341, 145], [320, 168], [329, 139], [323, 180], [320, 189], [288, 164], [298, 135], [295, 186], [290, 190], [257, 165], [265, 140], [265, 189], [262, 194], [224, 165], [233, 152], [237, 187], [236, 192]]</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A18" t="n">
+        <v>0</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[[278, 447], [321, 432], [356, 404], [381, 378], [400, 362], [325, 342], [346, 308], [358, 287], [366, 268], [298, 335], [303, 288], [305, 261], [304, 239], [274, 339], [265, 297], [260, 270], [254, 246], [251, 352], [234, 322], [224, 303], [215, 284]]</t>
+          <t>[[261, 278], [308, 265], [360, 230], [374, 184], [350, 158], [332, 179], [346, 148], [339, 189], [332, 196], [301, 174], [315, 145], [310, 197], [305, 196], [271, 175], [282, 152], [282, 199], [277, 200], [238, 176], [249, 164], [254, 196], [251, 200]]</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A19" t="n">
+        <v>0</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[[280, 445], [322, 429], [356, 401], [382, 377], [401, 360], [326, 341], [347, 306], [358, 286], [366, 267], [299, 333], [303, 287], [306, 259], [304, 237], [274, 337], [265, 295], [258, 269], [252, 246], [251, 351], [235, 321], [224, 301], [216, 283]]</t>
+          <t>[[270, 279], [317, 263], [368, 228], [384, 184], [361, 159], [340, 177], [356, 150], [346, 191], [339, 194], [309, 172], [325, 146], [318, 196], [313, 194], [280, 174], [292, 152], [291, 198], [287, 198], [247, 175], [258, 164], [262, 195], [260, 198]]</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A20" t="n">
+        <v>0</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[[280, 445], [322, 429], [357, 402], [381, 378], [401, 361], [325, 342], [346, 308], [358, 286], [367, 268], [298, 334], [303, 288], [305, 260], [304, 238], [274, 338], [265, 297], [258, 270], [253, 246], [251, 352], [235, 323], [225, 303], [216, 284]]</t>
+          <t>[[276, 280], [324, 269], [377, 236], [391, 191], [370, 164], [350, 184], [364, 154], [356, 195], [351, 202], [319, 178], [333, 150], [328, 201], [322, 201], [289, 179], [299, 155], [299, 202], [295, 204], [255, 179], [266, 166], [271, 199], [268, 204]]</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A21" t="n">
+        <v>0</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[[289, 504], [255, 470], [234, 425], [226, 384], [229, 354], [276, 422], [288, 364], [296, 335], [303, 318], [312, 432], [329, 371], [335, 342], [339, 325], [340, 439], [359, 387], [366, 358], [369, 339], [360, 444], [373, 401], [376, 376], [375, 357]]</t>
+          <t>[[277, 281], [325, 274], [380, 241], [396, 194], [371, 169], [355, 187], [369, 159], [360, 199], [354, 207], [323, 181], [337, 154], [330, 206], [325, 206], [292, 181], [303, 159], [302, 206], [297, 208], [259, 180], [269, 168], [274, 201], [271, 206]]</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A22" t="n">
+        <v>0</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[[262, 364], [233, 332], [212, 297], [196, 265], [179, 246], [257, 262], [255, 215], [254, 190], [254, 170], [284, 265], [301, 218], [312, 193], [322, 176], [306, 277], [334, 241], [352, 221], [366, 206], [322, 293], [349, 273], [364, 262], [377, 251]]</t>
+          <t>[[337, 332], [303, 306], [291, 277], [304, 256], [326, 252], [311, 237], [319, 237], [320, 251], [319, 260], [337, 236], [342, 243], [341, 256], [338, 266], [360, 243], [361, 255], [357, 266], [352, 275], [379, 255], [379, 268], [375, 279], [369, 286]]</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A23" t="n">
+        <v>0</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[[275, 371], [244, 342], [224, 308], [209, 277], [192, 258], [269, 271], [267, 226], [267, 204], [268, 185], [296, 273], [310, 229], [321, 206], [330, 191], [318, 285], [342, 250], [359, 231], [372, 217], [333, 302], [358, 283], [372, 272], [384, 263]]</t>
+          <t>[[351, 327], [316, 295], [305, 263], [319, 242], [341, 239], [326, 226], [337, 223], [339, 238], [337, 250], [354, 228], [361, 229], [359, 243], [355, 255], [379, 237], [378, 241], [376, 254], [371, 265], [398, 251], [396, 255], [392, 265], [386, 274]]</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A24" t="n">
+        <v>0</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[[278, 371], [249, 341], [230, 307], [214, 276], [198, 258], [274, 271], [271, 228], [270, 205], [271, 186], [299, 274], [315, 231], [326, 209], [334, 194], [321, 286], [345, 253], [361, 233], [373, 219], [336, 303], [360, 284], [373, 273], [384, 263]]</t>
+          <t>[[356, 322], [321, 302], [306, 274], [316, 252], [334, 245], [329, 231], [335, 232], [337, 245], [335, 254], [355, 230], [358, 237], [357, 250], [354, 261], [379, 238], [377, 249], [373, 261], [370, 271], [398, 251], [396, 262], [391, 273], [387, 281]]</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A25" t="n">
+        <v>0</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[[281, 371], [253, 340], [235, 305], [220, 274], [205, 255], [279, 270], [278, 227], [278, 204], [280, 186], [305, 274], [322, 232], [332, 210], [342, 195], [326, 287], [351, 254], [368, 235], [381, 221], [341, 304], [365, 284], [378, 274], [390, 265]]</t>
+          <t>[[358, 321], [322, 301], [307, 273], [316, 251], [334, 245], [328, 231], [336, 230], [338, 243], [336, 252], [355, 230], [358, 235], [358, 248], [356, 259], [379, 237], [378, 246], [375, 258], [372, 268], [399, 249], [397, 258], [393, 269], [389, 277]]</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A26" t="n">
+        <v>0</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[[282, 372], [254, 341], [237, 305], [224, 274], [208, 255], [282, 270], [282, 229], [282, 206], [284, 188], [308, 275], [324, 234], [335, 213], [344, 198], [328, 288], [353, 257], [370, 239], [383, 226], [342, 306], [365, 288], [377, 278], [388, 269]]</t>
+          <t>[[358, 321], [321, 300], [306, 272], [315, 249], [331, 241], [330, 229], [333, 226], [335, 239], [334, 249], [356, 229], [357, 232], [356, 245], [356, 256], [380, 236], [377, 244], [374, 255], [372, 265], [400, 248], [396, 256], [393, 266], [390, 275]]</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A27" t="n">
+        <v>0</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[[187, 439], [253, 411], [307, 364], [344, 319], [383, 292], [243, 255], [264, 185], [275, 141], [280, 101], [191, 247], [188, 167], [185, 115], [180, 70], [145, 263], [120, 189], [103, 137], [89, 92], [106, 296], [57, 249], [25, 216], [-1, 183]]</t>
+          <t>[[363, 327], [325, 303], [310, 271], [318, 247], [336, 242], [338, 229], [343, 232], [345, 246], [343, 256], [367, 231], [368, 239], [366, 252], [364, 263], [392, 242], [390, 252], [386, 262], [382, 273], [412, 257], [409, 265], [404, 276], [400, 284]]</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A28" t="n">
+        <v>0</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[[215, 457], [284, 430], [343, 380], [384, 334], [423, 303], [279, 264], [302, 192], [313, 146], [317, 104], [225, 256], [224, 171], [221, 119], [214, 74], [177, 271], [152, 195], [134, 144], [120, 98], [136, 304], [89, 254], [59, 220], [36, 186]]</t>
+          <t>[[367, 326], [329, 304], [312, 272], [319, 247], [337, 242], [339, 230], [341, 227], [343, 240], [342, 250], [367, 231], [366, 235], [365, 248], [365, 259], [392, 239], [388, 247], [384, 259], [382, 269], [412, 252], [408, 260], [404, 271], [400, 280]]</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A29" t="n">
+        <v>0</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[[222, 453], [292, 425], [352, 377], [392, 334], [428, 303], [287, 261], [309, 190], [320, 145], [325, 103], [233, 253], [232, 169], [228, 116], [221, 71], [185, 269], [158, 193], [140, 142], [125, 96], [144, 303], [98, 252], [69, 218], [45, 183]]</t>
+          <t>[[368, 328], [331, 306], [314, 274], [320, 249], [337, 243], [339, 232], [346, 227], [348, 240], [345, 251], [366, 231], [370, 236], [369, 250], [368, 261], [391, 239], [391, 248], [388, 259], [384, 270], [412, 251], [411, 259], [407, 271], [403, 280]]</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A30" t="n">
+        <v>0</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[[229, 451], [296, 424], [356, 377], [399, 335], [435, 304], [294, 262], [316, 190], [327, 145], [332, 103], [239, 253], [238, 168], [235, 115], [228, 69], [191, 268], [164, 192], [145, 141], [131, 95], [150, 301], [104, 250], [75, 217], [52, 182]]</t>
+          <t>[[374, 328], [337, 304], [321, 272], [326, 247], [343, 242], [348, 233], [346, 227], [349, 238], [351, 248], [375, 233], [373, 235], [372, 247], [371, 259], [400, 242], [394, 247], [391, 258], [389, 268], [419, 255], [413, 259], [409, 269], [407, 278]]</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A31" t="n">
+        <v>0</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[[502, 397], [552, 366], [578, 310], [599, 269], [624, 245], [532, 241], [543, 183], [546, 146], [544, 113], [501, 242], [489, 173], [481, 131], [468, 95], [477, 260], [454, 199], [437, 162], [418, 129], [460, 293], [436, 263], [419, 241], [401, 220]]</t>
+          <t>[[428, 401], [440, 365], [461, 349], [482, 355], [491, 368], [505, 343], [512, 354], [503, 361], [493, 362], [514, 367], [512, 376], [502, 380], [492, 380], [514, 391], [509, 399], [498, 401], [488, 400], [509, 413], [501, 418], [491, 419], [483, 416]]</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A32" t="n">
+        <v>0</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[[505, 398], [556, 367], [582, 310], [605, 268], [630, 243], [538, 241], [548, 184], [551, 147], [549, 114], [508, 242], [497, 175], [489, 132], [476, 96], [485, 262], [463, 201], [446, 163], [427, 128], [469, 295], [448, 265], [431, 242], [415, 218]]</t>
+          <t>[[439, 393], [445, 358], [465, 341], [486, 344], [496, 355], [511, 334], [512, 343], [503, 348], [495, 349], [520, 357], [516, 363], [507, 366], [498, 368], [521, 381], [515, 384], [505, 385], [496, 386], [516, 402], [510, 403], [501, 403], [493, 403]]</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A33" t="n">
+        <v>0</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[[507, 394], [556, 361], [581, 305], [604, 265], [628, 241], [538, 237], [548, 180], [551, 144], [550, 112], [509, 238], [499, 171], [491, 129], [479, 93], [487, 258], [466, 197], [450, 159], [432, 125], [472, 291], [450, 260], [434, 237], [417, 213]]</t>
+          <t>[[444, 395], [450, 360], [471, 344], [493, 352], [502, 367], [518, 340], [515, 350], [504, 355], [496, 356], [526, 366], [517, 373], [507, 375], [498, 377], [524, 391], [514, 397], [504, 396], [495, 395], [517, 412], [505, 417], [496, 416], [490, 413]]</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A34" t="n">
+        <v>0</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[[498, 393], [549, 361], [574, 304], [595, 264], [619, 239], [530, 235], [539, 178], [542, 141], [540, 108], [500, 236], [489, 168], [480, 125], [468, 89], [478, 256], [455, 195], [438, 157], [419, 122], [462, 289], [438, 258], [420, 236], [403, 213]]</t>
+          <t>[[447, 398], [451, 364], [471, 345], [491, 349], [500, 360], [519, 343], [518, 348], [509, 352], [502, 354], [527, 367], [521, 369], [511, 370], [503, 373], [526, 391], [519, 391], [509, 390], [500, 392], [519, 411], [513, 410], [505, 408], [498, 409]]</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A35" t="n">
+        <v>0</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[[299, 470], [270, 440], [250, 405], [232, 376], [212, 363], [295, 375], [288, 328], [284, 301], [283, 280], [321, 379], [331, 331], [339, 304], [347, 285], [341, 389], [362, 352], [378, 330], [391, 315], [356, 403], [379, 379], [394, 368], [407, 358]]</t>
+          <t>[[449, 404], [451, 367], [472, 348], [493, 352], [502, 363], [523, 348], [515, 352], [505, 356], [498, 359], [530, 373], [519, 375], [509, 376], [501, 380], [528, 398], [517, 397], [507, 396], [498, 398], [520, 418], [511, 417], [502, 415], [496, 415]]</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A36" t="n">
+        <v>0</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[[308, 470], [280, 440], [260, 405], [243, 375], [223, 362], [307, 376], [298, 328], [295, 301], [294, 279], [332, 380], [341, 331], [349, 305], [357, 286], [352, 389], [370, 351], [386, 330], [397, 314], [366, 402], [387, 376], [402, 365], [415, 356]]</t>
+          <t>[[446, 405], [450, 367], [472, 349], [494, 354], [503, 367], [522, 349], [513, 350], [502, 355], [496, 359], [529, 374], [518, 373], [507, 375], [500, 379], [527, 398], [516, 397], [506, 395], [497, 397], [519, 419], [512, 417], [503, 415], [496, 415]]</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A37" t="n">
+        <v>0</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[[311, 471], [282, 440], [263, 404], [245, 374], [226, 361], [309, 375], [301, 328], [298, 302], [298, 280], [334, 379], [343, 332], [352, 306], [360, 288], [354, 390], [372, 352], [387, 331], [399, 315], [368, 403], [389, 377], [403, 366], [416, 357]]</t>
+          <t>[[447, 405], [451, 367], [472, 348], [494, 355], [503, 368], [523, 350], [511, 350], [500, 355], [494, 359], [530, 375], [516, 373], [505, 375], [498, 380], [527, 399], [515, 397], [504, 396], [497, 398], [519, 419], [509, 417], [500, 415], [495, 415]]</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A38" t="n">
+        <v>0</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[[316, 468], [287, 438], [269, 401], [251, 372], [232, 358], [314, 373], [307, 326], [305, 299], [305, 279], [339, 377], [349, 331], [357, 306], [366, 288], [359, 387], [376, 350], [391, 330], [403, 315], [372, 401], [393, 377], [407, 366], [419, 357]]</t>
+          <t>[[459, 338], [472, 366], [497, 387], [521, 389], [532, 375], [517, 360], [536, 362], [513, 364], [504, 363], [515, 343], [533, 346], [505, 349], [499, 346], [510, 326], [527, 329], [501, 334], [494, 331], [504, 308], [515, 313], [498, 319], [491, 317]]</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A39" t="n">
+        <v>0</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[[319, 468], [289, 437], [271, 401], [254, 371], [235, 356], [318, 372], [311, 325], [309, 299], [309, 278], [343, 376], [352, 331], [361, 306], [369, 289], [362, 386], [380, 350], [396, 330], [408, 316], [376, 399], [398, 375], [414, 365], [428, 356]]</t>
+          <t>[[461, 335], [472, 362], [497, 382], [521, 384], [533, 372], [516, 357], [536, 357], [513, 360], [504, 360], [515, 339], [532, 342], [505, 346], [499, 343], [510, 323], [526, 326], [500, 331], [494, 329], [504, 305], [514, 310], [496, 316], [490, 313]]</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A40" t="n">
+        <v>0</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[[349, 411], [360, 371], [381, 343], [398, 318], [402, 297], [428, 367], [461, 345], [482, 335], [499, 328], [435, 390], [470, 385], [493, 384], [509, 386], [431, 410], [463, 415], [483, 420], [500, 426], [422, 426], [441, 436], [451, 442], [462, 448]]</t>
+          <t>[[459, 338], [470, 366], [496, 386], [520, 388], [532, 375], [516, 359], [536, 360], [514, 364], [505, 364], [514, 341], [532, 344], [504, 349], [499, 345], [509, 325], [526, 329], [500, 334], [494, 330], [503, 306], [514, 313], [495, 318], [490, 315]]</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A41" t="n">
+        <v>0</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[[350, 410], [360, 371], [382, 343], [399, 319], [404, 298], [428, 367], [461, 346], [481, 335], [499, 328], [435, 390], [471, 386], [494, 385], [511, 388], [432, 411], [464, 415], [484, 420], [500, 426], [423, 425], [442, 437], [453, 443], [464, 449]]</t>
+          <t>[[459, 339], [470, 365], [496, 385], [519, 387], [531, 375], [518, 359], [537, 361], [515, 364], [505, 363], [515, 342], [532, 344], [505, 349], [498, 345], [510, 325], [526, 329], [500, 335], [494, 331], [503, 307], [514, 314], [497, 319], [491, 316]]</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A42" t="n">
+        <v>0</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[[350, 414], [361, 376], [382, 347], [399, 323], [406, 305], [428, 372], [462, 350], [483, 340], [500, 334], [434, 395], [472, 391], [495, 391], [511, 393], [431, 415], [464, 421], [485, 426], [501, 431], [421, 431], [440, 443], [451, 449], [462, 455]]</t>
+          <t>[[457, 341], [470, 368], [496, 386], [519, 388], [531, 376], [516, 360], [535, 362], [512, 366], [502, 364], [513, 343], [531, 346], [503, 352], [497, 348], [508, 327], [525, 331], [499, 338], [492, 333], [502, 308], [514, 316], [496, 322], [490, 318]]</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A43" t="n">
+        <v>0</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[[351, 419], [361, 380], [383, 350], [401, 327], [411, 310], [431, 374], [465, 353], [485, 344], [502, 338], [437, 398], [474, 395], [496, 394], [512, 396], [434, 419], [465, 425], [485, 429], [501, 433], [424, 435], [442, 446], [453, 451], [463, 456]]</t>
+          <t>[[456, 344], [473, 368], [498, 382], [519, 383], [530, 371], [518, 355], [535, 360], [514, 365], [505, 362], [516, 339], [532, 346], [507, 352], [500, 346], [511, 324], [527, 333], [502, 339], [495, 332], [504, 307], [518, 320], [500, 326], [492, 320]]</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A44" t="n">
+        <v>0</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[[352, 419], [362, 380], [384, 351], [402, 328], [410, 309], [431, 375], [464, 355], [484, 345], [502, 339], [437, 399], [473, 395], [494, 394], [509, 396], [434, 420], [465, 424], [485, 429], [500, 433], [424, 435], [443, 446], [453, 452], [463, 458]]</t>
+          <t>[[161, 274], [204, 253], [240, 211], [249, 173], [231, 156], [208, 175], [206, 148], [207, 180], [209, 200], [179, 177], [176, 152], [180, 188], [182, 206], [151, 184], [148, 163], [155, 196], [158, 212], [124, 194], [124, 176], [131, 200], [135, 212]]</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A45" t="n">
+        <v>0</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[[318, 392], [343, 419], [374, 438], [400, 454], [418, 467], [411, 393], [447, 398], [468, 400], [486, 399], [410, 369], [449, 358], [471, 351], [487, 343], [399, 350], [426, 327], [443, 312], [458, 300], [381, 337], [397, 313], [406, 298], [417, 284]]</t>
+          <t>[[178, 240], [227, 214], [256, 182], [265, 145], [250, 123], [222, 145], [227, 112], [231, 146], [227, 167], [196, 146], [202, 115], [207, 157], [203, 176], [170, 152], [176, 123], [184, 163], [181, 180], [141, 161], [150, 137], [160, 165], [158, 179]]</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A46" t="n">
+        <v>0</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[[321, 395], [346, 422], [377, 440], [403, 457], [421, 471], [414, 394], [450, 400], [471, 403], [488, 402], [413, 370], [453, 359], [475, 353], [491, 345], [402, 352], [431, 329], [447, 314], [462, 302], [384, 340], [401, 316], [411, 300], [422, 287]]</t>
+          <t>[[173, 243], [222, 216], [252, 180], [262, 141], [246, 120], [220, 142], [224, 110], [227, 147], [226, 165], [192, 144], [196, 114], [203, 158], [199, 172], [165, 151], [172, 121], [180, 163], [177, 177], [136, 159], [145, 135], [155, 165], [153, 177]]</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A47" t="n">
+        <v>0</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[[322, 396], [346, 421], [376, 439], [402, 455], [420, 469], [414, 394], [450, 399], [471, 402], [488, 401], [413, 371], [453, 359], [474, 353], [490, 345], [402, 353], [431, 329], [448, 314], [462, 302], [384, 340], [399, 316], [409, 300], [420, 286]]</t>
+          <t>[[176, 251], [226, 236], [265, 205], [283, 166], [266, 142], [242, 160], [247, 128], [244, 165], [242, 180], [212, 157], [219, 128], [218, 173], [215, 183], [184, 160], [190, 134], [192, 176], [190, 188], [154, 162], [160, 145], [167, 175], [167, 185]]</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A48" t="n">
+        <v>0</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[[323, 396], [347, 421], [378, 439], [403, 456], [419, 471], [416, 395], [451, 400], [472, 403], [489, 402], [415, 371], [454, 359], [475, 351], [491, 343], [404, 354], [433, 330], [449, 315], [464, 303], [386, 342], [403, 318], [413, 302], [423, 288]]</t>
+          <t>[[187, 253], [235, 241], [275, 208], [293, 170], [279, 146], [251, 164], [259, 131], [256, 167], [252, 181], [222, 162], [231, 131], [230, 176], [225, 184], [194, 164], [202, 138], [204, 180], [201, 189], [163, 166], [173, 148], [179, 177], [176, 186]]</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A49" t="n">
+        <v>0</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[[323, 396], [346, 421], [376, 439], [400, 456], [417, 470], [416, 395], [451, 401], [472, 404], [489, 403], [415, 372], [454, 359], [475, 352], [491, 345], [404, 355], [432, 330], [449, 315], [464, 302], [385, 343], [401, 319], [411, 303], [422, 289]]</t>
+          <t>[[193, 259], [238, 245], [280, 210], [297, 173], [281, 150], [254, 162], [261, 134], [257, 173], [253, 183], [224, 161], [233, 136], [232, 182], [228, 185], [196, 164], [203, 144], [205, 185], [203, 188], [166, 167], [174, 155], [179, 183], [178, 189]]</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A50" t="n">
+        <v>0</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[[325, 396], [348, 422], [378, 441], [402, 458], [419, 472], [419, 398], [453, 404], [473, 407], [491, 406], [418, 375], [457, 364], [479, 357], [496, 350], [407, 357], [436, 331], [453, 317], [469, 304], [388, 345], [405, 321], [415, 306], [426, 293]]</t>
+          <t>[[244, 366], [224, 326], [227, 293], [247, 276], [267, 273], [232, 279], [260, 249], [259, 266], [249, 281], [259, 289], [281, 261], [279, 275], [269, 290], [283, 302], [296, 281], [293, 292], [284, 304], [302, 317], [308, 297], [303, 305], [297, 316]]</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A51" t="n">
+        <v>0</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[[466, 456], [495, 426], [513, 389], [529, 361], [547, 343], [454, 348], [441, 308], [428, 286], [414, 268], [427, 358], [398, 320], [376, 300], [355, 285], [409, 376], [376, 345], [354, 328], [332, 312], [399, 401], [365, 390], [344, 383], [324, 374]]</t>
+          <t>[[295, 266], [279, 229], [284, 200], [303, 188], [321, 190], [287, 168], [306, 166], [308, 178], [302, 187], [310, 173], [323, 177], [322, 188], [316, 196], [333, 183], [340, 190], [337, 201], [330, 208], [353, 197], [354, 204], [350, 214], [343, 221]]</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A52" t="n">
+        <v>0</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[[465, 459], [494, 429], [514, 392], [530, 364], [548, 346], [455, 352], [443, 312], [430, 289], [416, 270], [429, 360], [401, 322], [380, 301], [360, 285], [410, 378], [379, 346], [357, 328], [336, 312], [399, 402], [366, 390], [345, 382], [325, 372]]</t>
+          <t>[[312, 268], [288, 238], [288, 210], [304, 195], [321, 192], [297, 173], [312, 168], [317, 181], [314, 191], [323, 175], [334, 177], [335, 189], [331, 200], [347, 184], [352, 191], [350, 202], [344, 211], [367, 198], [369, 207], [364, 217], [358, 224]]</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A53" t="n">
+        <v>0</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[[452, 455], [482, 428], [503, 391], [521, 364], [539, 346], [447, 348], [433, 309], [421, 287], [408, 267], [420, 354], [394, 315], [374, 292], [354, 274], [401, 370], [370, 338], [348, 319], [327, 301], [388, 395], [355, 381], [335, 372], [315, 361]]</t>
+          <t>[[311, 267], [290, 235], [291, 207], [307, 192], [325, 191], [297, 172], [317, 166], [321, 178], [317, 189], [322, 173], [337, 176], [337, 188], [332, 198], [345, 182], [354, 189], [352, 201], [345, 210], [366, 196], [371, 205], [367, 216], [359, 224]]</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A54" t="n">
+        <v>0</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[[447, 458], [478, 431], [502, 396], [520, 370], [539, 352], [444, 355], [431, 317], [417, 296], [402, 277], [417, 361], [392, 322], [372, 299], [352, 280], [397, 376], [367, 344], [345, 325], [325, 307], [384, 400], [352, 385], [332, 376], [313, 365]]</t>
+          <t>[[315, 269], [293, 237], [295, 207], [314, 193], [334, 194], [304, 171], [318, 169], [321, 182], [317, 191], [329, 174], [339, 179], [338, 191], [334, 200], [353, 185], [357, 193], [354, 204], [348, 212], [372, 200], [372, 209], [368, 219], [362, 226]]</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A55" t="n">
+        <v>0</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[[399, 394], [435, 408], [467, 411], [493, 411], [512, 410], [476, 349], [505, 336], [523, 326], [536, 317], [469, 332], [499, 308], [517, 293], [529, 280], [457, 320], [478, 287], [492, 266], [503, 246], [440, 314], [452, 284], [459, 265], [466, 248]]</t>
+          <t>[[318, 271], [298, 237], [300, 208], [318, 195], [337, 196], [307, 176], [324, 168], [330, 180], [327, 191], [332, 179], [345, 179], [346, 191], [341, 201], [355, 189], [362, 194], [360, 205], [354, 213], [375, 203], [379, 209], [375, 220], [368, 227]]</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A56" t="n">
+        <v>0</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[[402, 402], [435, 417], [465, 420], [491, 419], [513, 418], [479, 358], [509, 345], [526, 336], [539, 327], [473, 341], [504, 317], [522, 303], [534, 290], [461, 329], [483, 296], [496, 275], [507, 256], [444, 322], [455, 292], [463, 274], [470, 258]]</t>
+          <t>[[319, 279], [301, 243], [305, 213], [323, 200], [341, 199], [316, 182], [330, 174], [332, 185], [328, 195], [340, 186], [350, 184], [349, 196], [344, 206], [363, 198], [367, 198], [363, 208], [358, 218], [381, 214], [381, 213], [377, 222], [371, 230]]</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A57" t="n">
+        <v>0</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[[244, 385], [285, 364], [317, 334], [338, 307], [355, 289], [278, 277], [290, 238], [295, 215], [296, 194], [250, 273], [246, 228], [243, 202], [237, 180], [226, 281], [210, 242], [199, 217], [189, 195], [204, 297], [181, 272], [165, 255], [153, 238]]</t>
+          <t>[[214, 258], [250, 248], [284, 232], [296, 204], [287, 185], [274, 203], [278, 179], [275, 189], [273, 197], [253, 197], [257, 173], [251, 202], [252, 213], [233, 194], [235, 174], [231, 204], [231, 216], [211, 193], [215, 178], [214, 200], [214, 211]]</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A58" t="n">
+        <v>0</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[[257, 389], [298, 370], [329, 340], [348, 314], [365, 297], [290, 283], [302, 245], [307, 221], [309, 200], [263, 279], [260, 234], [257, 207], [253, 185], [239, 286], [224, 246], [215, 220], [207, 199], [218, 301], [195, 275], [180, 257], [168, 240]]</t>
+          <t>[[227, 258], [262, 251], [298, 233], [311, 206], [302, 188], [288, 200], [294, 178], [290, 192], [287, 203], [267, 194], [272, 172], [266, 201], [266, 212], [247, 192], [249, 175], [246, 204], [246, 216], [223, 192], [229, 180], [229, 201], [230, 212]]</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A59" t="n">
+        <v>0</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[[262, 389], [303, 371], [336, 343], [356, 317], [372, 299], [298, 285], [311, 246], [315, 222], [317, 201], [271, 280], [270, 235], [268, 208], [263, 186], [247, 286], [235, 246], [225, 220], [216, 198], [226, 301], [205, 275], [191, 257], [180, 239]]</t>
+          <t>[[230, 258], [268, 248], [302, 231], [316, 205], [308, 188], [292, 201], [298, 175], [293, 192], [291, 205], [271, 195], [277, 171], [271, 201], [271, 211], [251, 192], [255, 174], [250, 205], [250, 215], [228, 192], [233, 178], [233, 200], [233, 209]]</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A60" t="n">
+        <v>0</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[[264, 389], [305, 371], [337, 342], [356, 316], [373, 299], [300, 285], [311, 246], [316, 222], [317, 200], [273, 280], [272, 236], [269, 208], [264, 186], [249, 287], [237, 246], [227, 220], [218, 198], [228, 302], [206, 275], [192, 257], [181, 239]]</t>
+          <t>[[239, 264], [276, 256], [314, 240], [327, 210], [314, 191], [303, 205], [311, 178], [303, 203], [301, 215], [282, 199], [289, 175], [282, 207], [280, 217], [261, 197], [265, 177], [261, 210], [260, 221], [237, 197], [242, 183], [243, 206], [243, 216]]</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A61" t="n">
+        <v>0</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[[271, 396], [314, 381], [345, 350], [364, 322], [381, 308], [308, 290], [321, 251], [325, 227], [327, 205], [281, 285], [279, 240], [277, 212], [272, 190], [256, 291], [243, 251], [235, 225], [227, 203], [236, 307], [213, 280], [200, 262], [188, 245]]</t>
+          <t>[[248, 272], [285, 264], [321, 248], [335, 220], [323, 201], [311, 211], [319, 186], [313, 211], [310, 223], [289, 205], [297, 182], [290, 216], [289, 225], [268, 204], [273, 186], [269, 218], [268, 228], [244, 204], [250, 190], [251, 214], [251, 223]]</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A62" t="n">
+        <v>0</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[[277, 404], [319, 388], [350, 357], [369, 329], [387, 313], [313, 297], [325, 257], [330, 232], [332, 210], [285, 292], [285, 246], [283, 217], [278, 194], [262, 298], [249, 257], [240, 230], [231, 207], [241, 314], [220, 286], [206, 268], [195, 250]]</t>
+          <t>[[455, 367], [458, 331], [478, 314], [499, 321], [507, 334], [524, 316], [514, 325], [503, 330], [497, 331], [533, 338], [520, 345], [509, 347], [502, 350], [533, 359], [519, 364], [508, 364], [501, 364], [527, 379], [514, 384], [504, 382], [498, 381]]</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A63" t="n">
+        <v>0</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[[208, 394], [180, 367], [162, 336], [145, 311], [125, 300], [198, 300], [193, 255], [190, 228], [189, 208], [222, 303], [236, 257], [245, 231], [253, 214], [243, 313], [267, 276], [283, 255], [295, 240], [259, 327], [284, 306], [298, 296], [309, 285]]</t>
+          <t>[[454, 371], [468, 330], [488, 311], [508, 313], [516, 325], [531, 320], [531, 320], [518, 324], [509, 328], [538, 344], [534, 341], [522, 341], [512, 344], [535, 367], [527, 359], [516, 359], [506, 362], [528, 385], [524, 379], [514, 377], [506, 377]]</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A64" t="n">
+        <v>0</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[[221, 392], [193, 365], [175, 334], [158, 309], [140, 297], [212, 298], [209, 254], [207, 227], [207, 207], [236, 301], [252, 257], [262, 233], [270, 215], [256, 312], [281, 277], [298, 258], [310, 243], [272, 326], [297, 308], [311, 298], [322, 287]]</t>
+          <t>[[464, 373], [466, 336], [486, 314], [506, 316], [515, 328], [533, 323], [522, 326], [513, 329], [508, 332], [540, 344], [528, 345], [518, 347], [511, 351], [539, 365], [526, 364], [516, 363], [510, 365], [533, 384], [522, 381], [514, 379], [508, 380]]</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A65" t="n">
+        <v>0</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[[229, 393], [203, 367], [185, 336], [169, 309], [150, 297], [224, 300], [223, 255], [221, 229], [222, 208], [248, 304], [264, 261], [275, 236], [284, 219], [268, 316], [293, 282], [310, 262], [322, 247], [283, 331], [308, 312], [322, 302], [334, 293]]</t>
+          <t>[[466, 374], [468, 335], [488, 314], [508, 317], [518, 330], [535, 324], [523, 324], [513, 328], [509, 331], [542, 346], [529, 343], [518, 345], [512, 349], [541, 367], [527, 362], [517, 361], [512, 364], [534, 384], [523, 379], [515, 378], [510, 379]]</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A66" t="n">
+        <v>0</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[[232, 398], [208, 368], [193, 335], [179, 307], [162, 295], [233, 303], [234, 258], [235, 231], [236, 211], [256, 308], [276, 266], [289, 243], [299, 227], [276, 321], [303, 287], [321, 269], [334, 254], [290, 336], [316, 319], [331, 309], [344, 300]]</t>
+          <t>[[459, 370], [471, 330], [491, 309], [510, 310], [516, 321], [534, 322], [534, 323], [521, 325], [511, 328], [541, 345], [537, 342], [524, 342], [514, 345], [538, 367], [529, 359], [518, 359], [508, 361], [531, 384], [525, 378], [516, 376], [507, 376]]</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A67" t="n">
+        <v>0</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[[236, 402], [212, 371], [196, 337], [183, 308], [166, 295], [237, 306], [236, 261], [236, 234], [237, 213], [260, 313], [280, 270], [292, 247], [302, 231], [279, 325], [306, 290], [324, 271], [337, 257], [293, 341], [321, 322], [336, 313], [349, 303]]</t>
+          <t>[[453, 331], [487, 354], [527, 364], [554, 363], [568, 352], [543, 345], [574, 344], [555, 350], [543, 351], [540, 324], [568, 323], [544, 331], [535, 330], [532, 304], [557, 306], [535, 315], [525, 313], [521, 283], [536, 290], [522, 300], [514, 300]]</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A68" t="n">
+        <v>0</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[[241, 374], [290, 361], [335, 332], [371, 309], [397, 293], [311, 255], [334, 214], [346, 188], [353, 165], [279, 244], [287, 190], [290, 157], [289, 131], [250, 247], [241, 196], [235, 163], [228, 135], [221, 262], [199, 225], [185, 201], [173, 177]]</t>
+          <t>[[513, 230], [536, 258], [562, 276], [588, 279], [599, 264], [570, 256], [590, 258], [581, 257], [573, 257], [568, 239], [588, 238], [570, 240], [559, 242], [563, 222], [582, 221], [560, 225], [546, 228], [555, 204], [570, 204], [555, 209], [543, 213]]</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A69" t="n">
+        <v>0</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[[235, 374], [284, 362], [329, 334], [362, 311], [389, 296], [303, 258], [326, 216], [338, 191], [345, 168], [271, 247], [279, 193], [282, 160], [280, 132], [241, 250], [234, 199], [226, 167], [219, 138], [213, 266], [191, 228], [176, 205], [165, 181]]</t>
+          <t>[[517, 222], [538, 250], [563, 269], [592, 271], [605, 257], [572, 253], [593, 256], [583, 254], [575, 252], [573, 234], [594, 234], [574, 235], [565, 236], [569, 216], [590, 215], [566, 219], [552, 221], [563, 198], [578, 199], [562, 204], [550, 206]]</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A70" t="n">
+        <v>0</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[[232, 376], [280, 363], [324, 335], [358, 311], [384, 295], [298, 260], [320, 218], [332, 192], [339, 169], [267, 249], [274, 196], [277, 163], [275, 135], [237, 253], [229, 202], [221, 169], [214, 140], [208, 268], [186, 231], [172, 207], [160, 184]]</t>
+          <t>[[518, 215], [539, 244], [565, 263], [592, 266], [606, 253], [576, 246], [598, 248], [588, 247], [578, 246], [576, 228], [597, 227], [577, 228], [565, 230], [573, 210], [592, 209], [568, 213], [554, 215], [566, 192], [581, 193], [564, 197], [553, 200]]</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A71" t="n">
+        <v>0</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[[233, 375], [281, 362], [323, 334], [357, 310], [384, 295], [298, 260], [320, 218], [332, 192], [339, 168], [267, 249], [275, 196], [278, 162], [277, 134], [238, 253], [230, 202], [223, 169], [216, 139], [210, 269], [188, 231], [174, 207], [162, 183]]</t>
+          <t>[[522, 207], [541, 235], [564, 253], [589, 257], [603, 245], [574, 238], [594, 243], [589, 240], [580, 237], [575, 221], [596, 222], [581, 220], [568, 221], [572, 204], [591, 204], [572, 204], [556, 206], [567, 187], [581, 188], [567, 190], [555, 193]]</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A72" t="n">
+        <v>0</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[[238, 392], [280, 372], [319, 335], [331, 298], [310, 279], [291, 284], [306, 259], [304, 297], [296, 304], [264, 283], [278, 262], [279, 308], [271, 307], [235, 287], [250, 275], [255, 315], [247, 316], [206, 294], [224, 287], [232, 315], [225, 319]]</t>
+          <t>[[514, 142], [538, 166], [565, 181], [590, 178], [596, 163], [569, 172], [590, 170], [579, 165], [569, 165], [565, 156], [585, 148], [567, 148], [556, 153], [560, 140], [576, 131], [558, 135], [547, 141], [553, 124], [566, 119], [553, 122], [545, 126]]</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A73" t="n">
+        <v>0</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[[233, 372], [273, 354], [311, 324], [326, 290], [308, 269], [290, 277], [303, 247], [299, 284], [292, 292], [263, 275], [275, 250], [274, 294], [268, 294], [235, 278], [246, 260], [249, 300], [244, 301], [206, 283], [220, 271], [226, 298], [221, 303]]</t>
+          <t>[[506, 112], [528, 133], [555, 146], [581, 139], [589, 124], [562, 136], [582, 135], [571, 130], [563, 129], [559, 119], [578, 113], [559, 115], [549, 120], [554, 104], [571, 96], [550, 102], [538, 108], [547, 88], [558, 83], [545, 89], [537, 93]]</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A74" t="n">
+        <v>0</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[[231, 355], [271, 340], [311, 308], [323, 273], [303, 254], [288, 264], [303, 235], [298, 272], [291, 279], [262, 262], [275, 236], [273, 279], [267, 281], [235, 264], [247, 244], [249, 284], [244, 286], [206, 268], [221, 255], [226, 282], [222, 287]]</t>
+          <t>[[524, 157], [534, 138], [547, 135], [562, 135], [571, 139], [556, 148], [571, 143], [565, 140], [558, 140], [562, 160], [579, 152], [570, 148], [564, 149], [569, 173], [584, 164], [577, 159], [570, 161], [576, 189], [591, 183], [588, 179], [585, 178]]</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A75" t="n">
+        <v>0</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[[235, 342], [277, 328], [317, 298], [328, 262], [309, 242], [292, 256], [307, 228], [302, 264], [296, 269], [268, 253], [280, 226], [278, 269], [272, 271], [242, 255], [253, 234], [254, 274], [249, 277], [213, 257], [227, 245], [232, 271], [226, 276]]</t>
+          <t>[[538, 219], [554, 249], [587, 267], [616, 264], [619, 244], [600, 242], [616, 244], [601, 248], [592, 249], [597, 225], [612, 225], [591, 231], [581, 232], [591, 208], [605, 207], [582, 217], [570, 219], [582, 191], [595, 192], [577, 200], [565, 202]]</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A76" t="n">
+        <v>0</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[[243, 344], [285, 328], [323, 298], [335, 264], [318, 246], [299, 258], [313, 229], [309, 264], [304, 271], [275, 255], [287, 228], [285, 269], [279, 272], [249, 256], [260, 235], [263, 273], [257, 277], [221, 259], [235, 245], [241, 270], [235, 276]]</t>
+          <t>[[543, 269], [562, 295], [597, 313], [624, 312], [635, 297], [606, 283], [625, 286], [627, 292], [623, 294], [602, 266], [624, 267], [602, 273], [585, 274], [595, 248], [617, 250], [593, 260], [575, 262], [583, 230], [603, 234], [587, 243], [572, 245]]</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A77" t="n">
+        <v>0</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[[104, 298], [136, 279], [170, 246], [175, 210], [155, 194], [153, 213], [147, 189], [148, 220], [152, 225], [126, 214], [119, 194], [125, 232], [129, 231], [101, 219], [95, 202], [102, 236], [107, 238], [76, 224], [73, 214], [81, 237], [86, 242]]</t>
+          <t>[[565, 284], [601, 302], [632, 305], [653, 299], [664, 292], [634, 272], [652, 267], [641, 278], [627, 283], [625, 258], [646, 255], [630, 268], [613, 272], [614, 246], [636, 242], [620, 256], [604, 262], [600, 234], [623, 232], [612, 245], [599, 251]]</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A78" t="n">
+        <v>0</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[[110, 298], [140, 284], [175, 249], [180, 212], [160, 195], [155, 213], [150, 190], [151, 222], [155, 229], [128, 216], [123, 196], [129, 234], [132, 234], [104, 220], [99, 203], [107, 238], [111, 240], [80, 224], [78, 215], [85, 239], [89, 243]]</t>
+          <t>[[610, 255], [622, 240], [632, 224], [642, 213], [651, 205], [615, 203], [636, 193], [650, 198], [656, 204], [615, 200], [637, 193], [649, 200], [654, 206], [617, 200], [640, 193], [650, 200], [656, 205], [621, 201], [640, 195], [650, 199], [655, 204]]</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A79" t="n">
+        <v>0</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[[117, 304], [148, 296], [187, 261], [192, 221], [171, 203], [168, 223], [162, 202], [162, 232], [167, 239], [140, 223], [135, 204], [139, 244], [144, 243], [116, 226], [110, 210], [117, 246], [122, 248], [90, 228], [87, 222], [94, 247], [99, 251]]</t>
+          <t>[[408, 260], [434, 249], [459, 227], [478, 208], [490, 193], [440, 194], [457, 177], [469, 184], [478, 194], [427, 191], [442, 175], [452, 187], [457, 198], [413, 192], [427, 175], [437, 188], [440, 200], [398, 195], [411, 181], [420, 190], [423, 200]]</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A80" t="n">
+        <v>0</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[[123, 307], [153, 295], [191, 259], [198, 222], [176, 204], [170, 223], [167, 201], [167, 233], [170, 239], [143, 223], [140, 204], [144, 244], [147, 243], [119, 227], [115, 211], [121, 246], [125, 247], [93, 229], [92, 223], [98, 247], [102, 250]]</t>
+          <t>[[235, 256], [267, 237], [290, 209], [301, 187], [304, 174], [275, 186], [281, 168], [282, 177], [283, 188], [261, 186], [262, 170], [264, 184], [267, 197], [247, 189], [248, 175], [249, 190], [251, 202], [233, 195], [236, 184], [237, 195], [239, 205]]</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A81" t="n">
+        <v>0</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[[547, 333], [587, 309], [603, 284], [614, 263], [609, 244], [571, 248], [590, 228], [594, 253], [584, 266], [558, 246], [583, 226], [586, 257], [573, 270], [542, 243], [573, 224], [574, 257], [559, 269], [522, 242], [555, 227], [560, 252], [549, 264]]</t>
+          <t>[[149, 279], [173, 259], [193, 234], [192, 210], [182, 203], [186, 226], [182, 203], [177, 220], [179, 230], [170, 227], [163, 208], [161, 230], [167, 237], [156, 231], [147, 217], [149, 239], [155, 244], [140, 236], [136, 225], [137, 240], [141, 247]]</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A82" t="n">
+        <v>0</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[[546, 320], [574, 296], [580, 271], [586, 250], [583, 235], [542, 236], [564, 224], [572, 245], [564, 260], [532, 234], [562, 222], [570, 249], [558, 264], [520, 234], [555, 223], [561, 251], [547, 265], [507, 237], [542, 228], [549, 249], [538, 261]]</t>
+          <t>[[277, 376], [257, 338], [259, 308], [275, 294], [292, 294], [264, 282], [281, 271], [283, 284], [279, 294], [287, 287], [299, 282], [299, 294], [293, 303], [308, 298], [314, 297], [312, 308], [306, 317], [326, 311], [329, 310], [325, 320], [318, 327]]</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A83" t="n">
+        <v>0</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[[563, 334], [590, 311], [596, 287], [602, 268], [601, 251], [551, 247], [580, 235], [588, 259], [579, 273], [541, 245], [577, 236], [586, 264], [575, 278], [531, 246], [572, 237], [579, 265], [565, 278], [523, 251], [561, 244], [567, 264], [556, 276]]</t>
+          <t>[[294, 341], [269, 307], [267, 279], [280, 265], [297, 264], [278, 251], [282, 248], [284, 261], [284, 271], [300, 252], [303, 254], [302, 265], [299, 275], [321, 261], [320, 264], [318, 275], [315, 284], [338, 272], [335, 275], [331, 284], [328, 292]]</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A84" t="n">
+        <v>0</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[[563, 341], [593, 317], [599, 297], [607, 277], [607, 259], [551, 260], [585, 248], [591, 272], [582, 284], [544, 257], [586, 249], [593, 276], [581, 288], [539, 256], [583, 248], [587, 277], [571, 289], [534, 256], [574, 252], [576, 273], [562, 284]]</t>
+          <t>[[308, 305], [280, 285], [272, 261], [284, 246], [302, 243], [285, 223], [295, 228], [297, 240], [293, 247], [308, 222], [314, 230], [313, 241], [311, 250], [329, 228], [332, 240], [328, 250], [324, 258], [347, 238], [349, 252], [345, 262], [340, 269]]</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A85" t="n">
+        <v>0</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[[332, 396], [303, 359], [297, 328], [308, 309], [325, 309], [321, 298], [331, 301], [333, 317], [328, 329], [345, 297], [353, 307], [350, 322], [344, 332], [368, 305], [372, 316], [367, 331], [361, 340], [388, 320], [391, 331], [385, 344], [379, 352]]</t>
+          <t>[[318, 305], [288, 287], [278, 262], [291, 246], [309, 244], [295, 224], [300, 226], [302, 237], [300, 245], [319, 224], [321, 230], [320, 240], [318, 250], [340, 232], [340, 240], [337, 249], [333, 258], [358, 243], [356, 252], [352, 262], [348, 268]]</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A86" t="n">
+        <v>0</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[[337, 378], [305, 353], [289, 323], [294, 300], [307, 303], [324, 289], [328, 294], [326, 308], [323, 317], [347, 291], [347, 302], [344, 314], [341, 324], [368, 301], [365, 312], [361, 323], [356, 332], [386, 315], [383, 323], [378, 333], [373, 341]]</t>
+          <t>[[324, 312], [296, 281], [291, 251], [305, 235], [323, 233], [304, 223], [316, 216], [320, 227], [318, 237], [328, 224], [338, 222], [336, 235], [331, 245], [350, 233], [353, 235], [350, 246], [344, 256], [367, 245], [368, 249], [364, 258], [357, 265]]</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A87" t="n">
+        <v>0</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[[339, 378], [307, 351], [293, 322], [298, 300], [311, 303], [327, 289], [329, 295], [327, 309], [324, 318], [351, 292], [350, 302], [346, 314], [343, 324], [372, 302], [368, 313], [363, 324], [358, 332], [389, 316], [385, 325], [380, 335], [376, 341]]</t>
+          <t>[[332, 301], [303, 283], [293, 259], [305, 243], [323, 242], [310, 221], [318, 224], [320, 236], [317, 244], [334, 221], [338, 228], [337, 239], [335, 249], [355, 228], [356, 238], [353, 249], [349, 257], [373, 239], [372, 250], [368, 259], [364, 266]]</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A88" t="n">
+        <v>0</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[[344, 378], [311, 351], [300, 322], [307, 303], [321, 304], [329, 290], [333, 296], [331, 311], [328, 321], [354, 293], [353, 303], [349, 316], [346, 325], [375, 303], [371, 314], [366, 325], [362, 333], [393, 317], [389, 326], [384, 335], [380, 341]]</t>
+          <t>[[334, 302], [304, 284], [294, 260], [307, 243], [325, 241], [311, 221], [320, 225], [322, 237], [319, 245], [335, 221], [340, 229], [339, 241], [336, 249], [356, 229], [358, 239], [354, 249], [350, 258], [373, 240], [374, 251], [369, 261], [365, 268]]</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A89" t="n">
+        <v>0</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[[385, 432], [362, 394], [362, 366], [377, 353], [394, 354], [399, 351], [392, 343], [385, 356], [381, 369], [424, 366], [419, 362], [410, 374], [405, 385], [443, 386], [437, 384], [428, 392], [420, 402], [456, 406], [451, 408], [441, 414], [435, 420]]</t>
+          <t>[[331, 309], [304, 279], [299, 252], [312, 237], [330, 235], [315, 218], [329, 217], [331, 231], [328, 241], [339, 221], [349, 223], [347, 236], [342, 246], [361, 232], [364, 236], [361, 247], [355, 257], [377, 245], [378, 251], [374, 260], [368, 268]]</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A90" t="n">
+        <v>0</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[[195, 349], [253, 323], [290, 290], [306, 249], [296, 225], [263, 266], [275, 237], [276, 248], [276, 255], [234, 262], [246, 238], [248, 254], [245, 261], [207, 262], [216, 240], [219, 257], [218, 268], [180, 264], [185, 241], [190, 253], [191, 262]]</t>
+          <t>[[344, 300], [317, 280], [312, 255], [327, 240], [345, 238], [326, 221], [337, 223], [337, 234], [333, 241], [350, 222], [357, 228], [355, 238], [351, 246], [372, 230], [374, 238], [370, 249], [366, 256], [389, 242], [389, 251], [384, 260], [380, 266]]</t>
         </is>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A91" t="n">
+        <v>0</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[[213, 324], [262, 304], [302, 263], [314, 218], [295, 197], [275, 222], [277, 185], [274, 224], [273, 238], [244, 221], [245, 187], [245, 235], [245, 243], [214, 225], [214, 194], [218, 240], [219, 252], [181, 231], [182, 207], [191, 240], [194, 253]]</t>
+          <t>[[346, 183], [388, 182], [425, 163], [441, 134], [426, 119], [407, 134], [420, 115], [413, 138], [408, 146], [391, 128], [403, 112], [395, 140], [388, 145], [373, 124], [384, 108], [377, 137], [370, 145], [351, 120], [363, 108], [359, 128], [354, 136]]</t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A92" t="n">
+        <v>0</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[[220, 331], [269, 321], [313, 278], [326, 232], [306, 213], [285, 232], [285, 199], [282, 239], [282, 253], [252, 232], [252, 200], [253, 248], [253, 258], [222, 235], [220, 206], [225, 253], [227, 265], [189, 239], [190, 222], [198, 256], [202, 266]]</t>
+          <t>[[351, 154], [393, 152], [424, 132], [436, 104], [421, 89], [404, 108], [413, 91], [412, 107], [409, 116], [388, 101], [402, 82], [397, 107], [389, 118], [372, 95], [386, 77], [381, 105], [373, 118], [350, 92], [366, 76], [365, 96], [359, 109]]</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A93" t="n">
+        <v>0</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[[224, 338], [273, 322], [316, 283], [327, 237], [307, 216], [287, 238], [290, 203], [286, 244], [286, 255], [255, 237], [258, 205], [258, 253], [257, 258], [226, 241], [227, 211], [231, 257], [231, 265], [193, 245], [195, 225], [203, 257], [206, 267]]</t>
+          <t>[[326, 155], [367, 152], [398, 132], [409, 106], [395, 93], [381, 111], [389, 91], [389, 103], [386, 114], [365, 105], [375, 85], [371, 105], [365, 117], [348, 100], [358, 81], [354, 103], [348, 116], [328, 98], [338, 81], [338, 96], [334, 107]]</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A94" t="n">
+        <v>0</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[[334, 424], [367, 413], [395, 386], [407, 359], [391, 348], [375, 358], [382, 340], [379, 365], [376, 373], [357, 356], [364, 339], [361, 370], [358, 374], [338, 357], [346, 341], [346, 371], [342, 377], [317, 359], [327, 346], [329, 367], [326, 374]]</t>
+          <t>[[299, 159], [341, 154], [374, 135], [387, 109], [379, 96], [362, 113], [370, 92], [364, 106], [361, 118], [344, 107], [353, 88], [345, 110], [342, 121], [326, 103], [334, 85], [327, 109], [323, 122], [305, 100], [315, 85], [311, 102], [308, 112]]</t>
         </is>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A95" t="n">
+        <v>0</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[[341, 418], [373, 408], [399, 382], [410, 357], [397, 346], [380, 357], [386, 337], [383, 361], [381, 368], [362, 355], [369, 336], [367, 365], [363, 369], [343, 357], [351, 339], [351, 367], [347, 373], [323, 358], [331, 344], [335, 363], [333, 371]]</t>
+          <t>[[157, 192], [191, 178], [218, 155], [224, 124], [210, 114], [212, 141], [221, 118], [209, 132], [203, 143], [194, 137], [195, 115], [188, 140], [191, 150], [176, 135], [174, 118], [170, 144], [173, 156], [157, 134], [155, 121], [154, 139], [156, 149]]</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A96" t="n">
+        <v>0</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[[343, 418], [375, 408], [402, 383], [412, 357], [397, 346], [381, 356], [389, 337], [386, 362], [382, 369], [363, 355], [371, 337], [369, 367], [365, 372], [345, 356], [353, 339], [354, 367], [350, 375], [324, 359], [333, 344], [338, 364], [336, 373]]</t>
+          <t>[[157, 193], [190, 182], [217, 158], [223, 127], [208, 117], [210, 145], [217, 123], [207, 137], [202, 148], [191, 141], [194, 118], [186, 142], [188, 155], [174, 139], [173, 121], [169, 147], [172, 160], [155, 138], [154, 125], [153, 143], [155, 154]]</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A97" t="n">
+        <v>0</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>[[343, 419], [374, 410], [401, 385], [412, 359], [398, 348], [382, 359], [388, 339], [385, 362], [382, 371], [364, 357], [370, 339], [368, 368], [365, 373], [345, 358], [352, 341], [353, 369], [349, 376], [325, 361], [333, 346], [337, 365], [335, 374]]</t>
+          <t>[[166, 187], [200, 176], [228, 155], [235, 128], [225, 116], [223, 141], [229, 120], [218, 131], [213, 141], [205, 137], [206, 116], [198, 136], [201, 147], [188, 136], [184, 119], [180, 142], [183, 153], [169, 135], [167, 122], [165, 137], [167, 147]]</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A98" t="n">
+        <v>0</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[[347, 428], [379, 419], [408, 397], [418, 373], [406, 361], [391, 367], [399, 349], [396, 372], [392, 381], [373, 364], [381, 350], [378, 377], [373, 383], [354, 364], [362, 350], [361, 378], [357, 385], [332, 366], [343, 354], [345, 373], [342, 381]]</t>
+          <t>[[181, 189], [216, 178], [244, 154], [250, 125], [236, 114], [240, 143], [249, 121], [237, 131], [232, 143], [222, 137], [226, 115], [216, 135], [216, 147], [204, 135], [204, 117], [197, 139], [199, 152], [185, 134], [186, 120], [183, 134], [183, 144]]</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A99" t="n">
+        <v>0</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[[286, 429], [235, 377], [216, 321], [223, 277], [246, 271], [256, 278], [267, 248], [263, 267], [257, 288], [297, 283], [298, 261], [292, 280], [287, 299], [333, 297], [322, 282], [317, 297], [312, 313], [362, 315], [346, 302], [339, 315], [336, 329]]</t>
+          <t>[[198, 190], [234, 178], [264, 156], [274, 127], [260, 116], [259, 142], [269, 121], [257, 130], [250, 141], [240, 136], [247, 114], [235, 135], [235, 147], [222, 133], [224, 115], [216, 139], [218, 152], [202, 130], [204, 118], [202, 134], [203, 144]]</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A100" t="n">
+        <v>0</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[[300, 414], [248, 360], [228, 302], [237, 260], [265, 261], [281, 261], [279, 234], [273, 255], [270, 276], [324, 268], [311, 247], [301, 264], [299, 286], [357, 284], [337, 268], [328, 280], [325, 299], [381, 304], [361, 288], [353, 299], [351, 316]]</t>
+          <t>[[294, 310], [276, 275], [279, 250], [297, 240], [314, 243], [280, 232], [297, 225], [298, 235], [294, 242], [302, 237], [313, 230], [312, 239], [307, 248], [322, 246], [325, 242], [323, 250], [319, 259], [339, 257], [336, 254], [333, 262], [330, 269]]</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A101" t="n">
+        <v>0</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[[311, 396], [259, 346], [240, 290], [248, 247], [273, 245], [292, 248], [289, 224], [284, 243], [283, 261], [333, 256], [319, 240], [310, 255], [309, 273], [367, 273], [346, 261], [338, 272], [334, 290], [390, 294], [369, 282], [361, 294], [358, 310]]</t>
+          <t>[[308, 290], [291, 260], [293, 238], [309, 228], [324, 229], [289, 216], [310, 215], [311, 226], [304, 233], [309, 216], [324, 221], [324, 231], [319, 237], [329, 222], [339, 228], [337, 239], [331, 246], [348, 232], [353, 238], [350, 248], [344, 255]]</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A102" t="n">
+        <v>0</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>[[318, 393], [266, 342], [247, 287], [257, 244], [283, 242], [300, 245], [295, 223], [290, 243], [290, 262], [340, 252], [325, 238], [317, 256], [316, 274], [373, 268], [352, 258], [343, 271], [341, 289], [396, 288], [375, 277], [367, 290], [365, 306]]</t>
+          <t>[[323, 280], [301, 258], [299, 237], [312, 225], [328, 224], [304, 211], [317, 213], [318, 224], [314, 231], [324, 210], [334, 217], [333, 227], [329, 234], [344, 215], [350, 224], [348, 234], [342, 241], [362, 225], [365, 235], [362, 245], [357, 250]]</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A103" t="n">
+        <v>0</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>[[241, 411], [294, 372], [335, 311], [351, 258], [324, 232], [302, 265], [296, 219], [296, 265], [296, 292], [264, 269], [258, 230], [265, 286], [267, 305], [228, 282], [222, 247], [235, 300], [241, 319], [191, 299], [189, 273], [203, 312], [210, 329]]</t>
+          <t>[[332, 279], [309, 259], [305, 238], [317, 225], [333, 223], [314, 206], [325, 212], [326, 224], [321, 231], [336, 206], [342, 215], [341, 226], [337, 234], [356, 213], [359, 224], [355, 234], [351, 241], [373, 224], [373, 236], [370, 245], [365, 250]]</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A104" t="n">
+        <v>0</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>[[246, 393], [303, 370], [353, 304], [365, 245], [335, 219], [313, 249], [311, 206], [311, 258], [310, 279], [272, 252], [272, 214], [277, 275], [276, 288], [234, 262], [234, 227], [245, 285], [245, 297], [194, 273], [200, 252], [212, 291], [214, 300]]</t>
+          <t>[[333, 280], [309, 260], [305, 239], [317, 226], [333, 224], [316, 206], [326, 211], [327, 223], [323, 230], [337, 206], [343, 215], [342, 226], [339, 233], [357, 213], [360, 225], [356, 235], [351, 241], [373, 224], [375, 237], [371, 246], [366, 251]]</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A105" t="n">
+        <v>0</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>[[256, 401], [310, 375], [358, 311], [372, 256], [346, 233], [317, 254], [320, 214], [321, 268], [317, 284], [277, 258], [282, 222], [289, 284], [284, 290], [240, 268], [244, 236], [257, 293], [254, 300], [201, 280], [210, 262], [223, 299], [222, 306]]</t>
+          <t>[[336, 282], [312, 261], [309, 239], [322, 226], [338, 225], [320, 208], [329, 212], [331, 225], [327, 233], [343, 210], [348, 217], [347, 228], [344, 236], [363, 218], [366, 227], [362, 237], [357, 245], [379, 231], [379, 242], [374, 251], [370, 256]]</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A106" t="n">
+        <v>0</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>[[256, 404], [310, 379], [358, 319], [374, 265], [350, 238], [319, 261], [321, 219], [320, 270], [317, 289], [280, 263], [282, 227], [288, 286], [285, 295], [243, 273], [245, 241], [256, 295], [256, 303], [204, 284], [211, 265], [224, 300], [225, 308]]</t>
+          <t>[[353, 280], [331, 259], [329, 238], [343, 226], [359, 227], [340, 212], [351, 215], [351, 227], [346, 234], [361, 213], [369, 220], [367, 230], [363, 238], [379, 220], [385, 228], [381, 238], [376, 246], [396, 231], [398, 241], [393, 250], [389, 255]]</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A107" t="n">
+        <v>0</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>[[161, 353], [128, 311], [119, 276], [135, 254], [160, 248], [119, 248], [143, 223], [148, 235], [143, 249], [150, 246], [167, 229], [170, 242], [164, 256], [181, 251], [186, 242], [187, 254], [182, 267], [208, 260], [205, 256], [203, 267], [198, 279]]</t>
+          <t>[[268, 410], [302, 397], [328, 373], [340, 348], [333, 330], [308, 344], [318, 325], [315, 344], [309, 355], [290, 342], [300, 324], [298, 347], [293, 358], [272, 343], [282, 328], [283, 349], [280, 359], [252, 345], [264, 335], [268, 349], [267, 357]]</t>
         </is>
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A108" t="n">
+        <v>0</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>[[169, 343], [136, 301], [128, 266], [143, 245], [165, 237], [136, 238], [156, 215], [160, 227], [155, 240], [166, 236], [180, 224], [181, 237], [175, 250], [194, 242], [198, 238], [197, 251], [191, 263], [219, 253], [216, 251], [214, 262], [209, 273]]</t>
+          <t>[[297, 366], [333, 358], [356, 341], [367, 321], [364, 304], [343, 314], [350, 294], [347, 313], [342, 326], [327, 311], [335, 290], [332, 313], [326, 325], [309, 309], [319, 289], [317, 314], [312, 325], [289, 309], [301, 293], [302, 310], [298, 320]]</t>
         </is>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A109" t="n">
+        <v>0</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>[[178, 337], [148, 298], [142, 263], [158, 243], [179, 237], [153, 234], [174, 216], [178, 227], [172, 239], [182, 234], [196, 227], [197, 239], [191, 250], [210, 242], [214, 241], [213, 252], [207, 264], [233, 255], [234, 254], [231, 264], [225, 275]]</t>
+          <t>[[302, 365], [337, 358], [359, 343], [369, 322], [366, 306], [345, 315], [353, 296], [350, 315], [344, 328], [330, 311], [339, 291], [335, 316], [329, 328], [313, 310], [324, 290], [322, 315], [316, 327], [294, 310], [306, 294], [307, 311], [304, 322]]</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A110" t="n">
+        <v>0</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>[[191, 336], [161, 297], [157, 263], [173, 242], [195, 238], [168, 236], [185, 217], [189, 228], [184, 239], [196, 237], [207, 229], [208, 241], [203, 251], [223, 245], [224, 243], [223, 254], [219, 264], [246, 258], [243, 256], [240, 265], [235, 274]]</t>
+          <t>[[309, 361], [342, 355], [365, 338], [374, 317], [371, 300], [350, 310], [360, 291], [358, 310], [351, 324], [336, 307], [346, 286], [343, 311], [336, 324], [319, 305], [329, 286], [328, 312], [322, 324], [299, 306], [311, 291], [313, 309], [309, 319]]</t>
         </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A111" t="n">
+        <v>0</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>[[561, 344], [593, 313], [607, 285], [613, 259], [604, 242], [575, 264], [591, 247], [592, 267], [581, 277], [561, 262], [582, 244], [583, 270], [570, 280], [544, 260], [568, 243], [570, 271], [555, 280], [525, 261], [552, 246], [556, 265], [545, 274]]</t>
+          <t>[[121, 391], [140, 381], [161, 358], [163, 337], [154, 327], [148, 337], [135, 324], [134, 341], [139, 348], [132, 340], [118, 329], [122, 349], [130, 353], [120, 343], [106, 335], [111, 353], [120, 357], [109, 347], [97, 341], [101, 356], [110, 361]]</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A112" t="n">
+        <v>0</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>[[559, 326], [594, 306], [608, 280], [617, 257], [606, 242], [579, 256], [593, 238], [598, 260], [591, 274], [565, 254], [582, 236], [587, 266], [574, 278], [547, 253], [569, 235], [574, 267], [559, 278], [526, 253], [553, 239], [559, 261], [547, 272]]</t>
+          <t>[[123, 389], [144, 379], [164, 356], [166, 336], [154, 327], [150, 333], [137, 326], [139, 343], [145, 347], [134, 335], [122, 330], [128, 350], [135, 351], [121, 339], [110, 335], [115, 354], [123, 355], [108, 344], [99, 342], [105, 355], [112, 358]]</t>
         </is>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A113" t="n">
+        <v>0</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>[[546, 319], [580, 301], [596, 276], [604, 251], [591, 237], [567, 251], [580, 232], [586, 254], [579, 270], [553, 249], [569, 231], [574, 261], [562, 274], [536, 248], [557, 230], [561, 262], [546, 274], [514, 248], [540, 233], [546, 254], [535, 266]]</t>
+          <t>[[125, 391], [144, 382], [165, 361], [169, 338], [157, 327], [152, 338], [140, 326], [141, 343], [147, 348], [136, 339], [125, 328], [129, 349], [136, 352], [123, 342], [111, 334], [116, 353], [124, 356], [110, 346], [101, 342], [105, 355], [113, 359]]</t>
         </is>
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A114" t="n">
+        <v>0</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>[[556, 331], [586, 313], [601, 289], [609, 266], [599, 249], [572, 260], [586, 244], [592, 266], [586, 280], [558, 258], [576, 242], [581, 271], [571, 284], [540, 257], [564, 243], [568, 274], [555, 286], [519, 259], [547, 247], [553, 268], [543, 279]]</t>
+          <t>[[271, 406], [323, 375], [365, 331], [381, 291], [363, 270], [334, 286], [339, 257], [340, 294], [338, 309], [300, 289], [306, 262], [310, 309], [308, 323], [266, 298], [274, 280], [283, 326], [282, 340], [233, 311], [243, 296], [253, 328], [253, 341]]</t>
         </is>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A115" t="n">
+        <v>0</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>[[555, 337], [584, 318], [599, 293], [608, 270], [599, 253], [568, 263], [585, 246], [590, 270], [583, 283], [554, 261], [576, 245], [581, 275], [569, 287], [537, 260], [564, 247], [568, 278], [553, 288], [518, 263], [549, 252], [554, 273], [542, 283]]</t>
+          <t>[[280, 341], [333, 322], [377, 282], [397, 239], [381, 209], [348, 235], [353, 198], [351, 234], [349, 257], [317, 234], [322, 201], [321, 250], [319, 271], [284, 240], [288, 215], [292, 263], [292, 282], [250, 249], [256, 229], [263, 263], [265, 279]]</t>
         </is>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A116" t="n">
+        <v>0</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>[[250, 365], [302, 351], [340, 297], [350, 245], [345, 211], [312, 246], [315, 202], [315, 246], [313, 270], [279, 248], [284, 210], [286, 263], [283, 279], [247, 253], [250, 226], [255, 277], [256, 290], [213, 260], [220, 237], [227, 273], [227, 286]]</t>
+          <t>[[290, 316], [353, 290], [398, 248], [419, 201], [405, 168], [368, 197], [378, 155], [376, 197], [370, 223], [335, 195], [345, 154], [346, 208], [340, 233], [302, 199], [312, 167], [316, 220], [313, 242], [264, 207], [278, 181], [286, 218], [284, 237]]</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A117" t="n">
+        <v>0</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>[[256, 360], [310, 344], [348, 290], [356, 238], [350, 202], [319, 240], [322, 195], [325, 241], [322, 261], [286, 242], [290, 204], [296, 259], [292, 269], [253, 247], [257, 220], [265, 271], [264, 279], [218, 254], [226, 232], [235, 268], [234, 279]]</t>
+          <t>[[294, 312], [356, 288], [401, 248], [424, 202], [411, 169], [371, 195], [384, 154], [380, 196], [373, 222], [339, 193], [351, 154], [350, 208], [344, 232], [306, 197], [317, 166], [321, 219], [317, 242], [269, 205], [282, 180], [291, 218], [289, 237]]</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A118" t="n">
+        <v>0</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>[[261, 364], [316, 343], [354, 292], [361, 243], [355, 206], [324, 242], [327, 197], [329, 241], [326, 263], [291, 243], [295, 205], [300, 258], [296, 272], [259, 248], [262, 221], [269, 271], [268, 281], [224, 255], [231, 234], [240, 269], [240, 281]]</t>
+          <t>[[362, 271], [321, 243], [310, 205], [321, 180], [339, 178], [334, 165], [328, 168], [331, 187], [333, 200], [364, 165], [357, 171], [356, 188], [356, 202], [390, 174], [381, 185], [376, 200], [374, 211], [411, 189], [401, 202], [395, 214], [393, 223]]</t>
         </is>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A119" t="n">
+        <v>0</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>[[263, 364], [318, 345], [355, 293], [363, 244], [359, 208], [326, 243], [330, 199], [332, 243], [329, 264], [293, 244], [298, 207], [303, 259], [299, 272], [260, 249], [265, 223], [271, 272], [270, 281], [226, 256], [235, 236], [242, 269], [240, 280]]</t>
+          <t>[[373, 282], [327, 256], [309, 211], [308, 176], [315, 172], [347, 170], [331, 174], [329, 191], [332, 201], [377, 173], [358, 178], [355, 193], [357, 205], [401, 186], [383, 188], [378, 200], [378, 212], [419, 201], [403, 201], [398, 212], [398, 222]]</t>
         </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A120" t="n">
+        <v>0</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>[[265, 364], [319, 343], [356, 293], [364, 245], [358, 209], [326, 243], [331, 200], [333, 243], [330, 265], [294, 244], [300, 208], [304, 260], [300, 273], [261, 249], [267, 223], [273, 272], [271, 281], [226, 256], [237, 236], [244, 269], [242, 280]]</t>
+          <t>[[372, 288], [324, 261], [303, 216], [299, 178], [308, 173], [345, 171], [323, 176], [320, 195], [324, 207], [375, 173], [351, 181], [346, 197], [349, 209], [399, 186], [377, 191], [371, 204], [372, 217], [417, 202], [398, 203], [392, 214], [394, 225]]</t>
         </is>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A121" t="n">
+        <v>0</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>[[317, 398], [293, 361], [290, 326], [302, 304], [315, 300], [323, 308], [337, 297], [331, 309], [323, 319], [351, 321], [356, 313], [348, 321], [342, 332], [373, 339], [375, 329], [367, 335], [361, 346], [390, 357], [387, 349], [379, 355], [373, 363]]</t>
+          <t>[[381, 299], [325, 268], [301, 215], [294, 169], [303, 161], [351, 161], [327, 160], [323, 182], [329, 196], [387, 166], [358, 169], [352, 187], [356, 201], [416, 182], [389, 183], [381, 197], [383, 211], [438, 202], [415, 198], [409, 211], [412, 223]]</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A122" t="n">
+        <v>0</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>[[308, 319], [273, 293], [256, 259], [262, 233], [278, 232], [290, 219], [300, 222], [299, 237], [293, 246], [317, 221], [322, 229], [319, 244], [313, 255], [341, 232], [339, 243], [335, 255], [329, 264], [360, 246], [357, 255], [351, 265], [346, 273]]</t>
+          <t>[[392, 319], [329, 284], [301, 226], [296, 174], [308, 166], [356, 169], [334, 160], [331, 183], [336, 199], [396, 172], [367, 172], [361, 191], [365, 207], [427, 188], [400, 187], [392, 202], [394, 219], [451, 207], [426, 202], [420, 217], [422, 233]]</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A123" t="n">
+        <v>0</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>[[311, 327], [276, 301], [259, 266], [265, 240], [280, 241], [296, 227], [302, 232], [300, 248], [296, 257], [322, 230], [323, 238], [320, 253], [316, 264], [346, 240], [342, 251], [337, 263], [332, 273], [365, 256], [359, 265], [354, 275], [349, 284]]</t>
+          <t>[[384, 327], [319, 289], [293, 230], [287, 177], [299, 168], [349, 170], [327, 168], [324, 191], [329, 206], [390, 174], [361, 178], [355, 198], [359, 214], [423, 192], [395, 193], [387, 210], [389, 227], [449, 214], [424, 210], [417, 225], [419, 240]]</t>
         </is>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A124" t="n">
+        <v>0</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>[[319, 324], [283, 297], [269, 265], [274, 240], [289, 240], [301, 228], [311, 227], [310, 241], [305, 252], [328, 231], [333, 235], [329, 249], [325, 260], [352, 241], [351, 248], [347, 259], [342, 269], [372, 255], [368, 262], [363, 272], [358, 280]]</t>
+          <t>[[400, 339], [338, 300], [310, 237], [305, 182], [319, 175], [358, 183], [346, 172], [345, 193], [349, 210], [399, 185], [379, 184], [375, 203], [379, 219], [435, 199], [412, 198], [406, 214], [406, 231], [463, 217], [441, 214], [435, 229], [436, 244]]</t>
         </is>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A125" t="n">
+        <v>0</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>[[324, 327], [290, 300], [276, 266], [282, 242], [296, 243], [312, 229], [316, 233], [315, 247], [311, 256], [339, 233], [338, 241], [334, 254], [331, 264], [362, 244], [357, 253], [352, 264], [348, 273], [380, 259], [374, 267], [368, 277], [364, 284]]</t>
+          <t>[[127, 313], [159, 300], [189, 276], [202, 249], [191, 235], [177, 254], [174, 229], [166, 246], [166, 257], [157, 254], [151, 231], [148, 257], [154, 266], [138, 255], [132, 237], [131, 263], [137, 273], [120, 257], [114, 246], [115, 264], [122, 273]]</t>
         </is>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A126" t="n">
+        <v>0</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>[[230, 372], [288, 343], [331, 280], [348, 224], [328, 190], [298, 230], [298, 182], [297, 234], [295, 254], [259, 233], [259, 194], [263, 254], [263, 263], [221, 242], [221, 211], [230, 267], [233, 275], [182, 251], [187, 230], [196, 269], [198, 280]]</t>
+          <t>[[139, 305], [172, 294], [203, 271], [216, 244], [204, 230], [191, 249], [189, 224], [181, 241], [181, 252], [170, 247], [167, 224], [163, 249], [168, 259], [152, 248], [147, 230], [146, 257], [151, 267], [133, 250], [129, 237], [130, 255], [135, 265]]</t>
         </is>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A127" t="n">
+        <v>0</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>[[238, 362], [294, 336], [336, 275], [353, 219], [333, 184], [300, 220], [303, 173], [304, 224], [301, 246], [262, 224], [266, 185], [272, 246], [268, 257], [224, 233], [228, 203], [239, 258], [238, 267], [186, 244], [193, 220], [205, 258], [204, 270]]</t>
+          <t>[[149, 300], [182, 289], [213, 267], [226, 241], [215, 226], [200, 245], [199, 220], [193, 239], [193, 250], [180, 243], [178, 220], [174, 247], [179, 256], [161, 244], [158, 226], [157, 253], [161, 263], [143, 245], [139, 233], [140, 252], [145, 261]]</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A128" t="n">
+        <v>0</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>[[248, 357], [304, 329], [344, 268], [359, 212], [336, 180], [310, 215], [313, 171], [314, 224], [311, 240], [271, 219], [274, 183], [281, 243], [277, 248], [234, 228], [238, 199], [248, 253], [246, 258], [196, 238], [204, 220], [215, 256], [212, 264]]</t>
+          <t>[[158, 303], [193, 292], [224, 268], [237, 242], [223, 228], [209, 245], [208, 220], [204, 240], [204, 252], [189, 243], [186, 220], [185, 249], [189, 258], [170, 244], [167, 226], [168, 255], [172, 266], [151, 247], [148, 234], [151, 254], [155, 264]]</t>
         </is>
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A129" t="n">
+        <v>0</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>[[259, 358], [315, 331], [353, 270], [369, 216], [349, 183], [318, 217], [322, 174], [324, 225], [321, 241], [281, 222], [285, 187], [292, 244], [287, 249], [245, 231], [250, 202], [260, 255], [257, 259], [209, 241], [218, 221], [227, 258], [223, 266]]</t>
+          <t>[[390, 252], [432, 239], [470, 218], [491, 193], [488, 169], [456, 170], [470, 153], [469, 178], [463, 186], [432, 165], [447, 149], [444, 181], [437, 185], [405, 165], [421, 152], [419, 185], [410, 190], [375, 168], [392, 160], [394, 183], [387, 189]]</t>
         </is>
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A130" t="n">
+        <v>0</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>[[111, 362], [155, 352], [196, 312], [213, 268], [197, 243], [177, 270], [173, 237], [169, 274], [171, 289], [144, 269], [141, 239], [141, 284], [144, 290], [116, 270], [113, 243], [114, 286], [118, 295], [85, 270], [84, 253], [87, 285], [92, 294]]</t>
+          <t>[[374, 159], [429, 150], [464, 128], [485, 97], [477, 74], [448, 88], [460, 59], [453, 86], [445, 105], [425, 81], [436, 52], [429, 89], [421, 107], [399, 78], [412, 51], [407, 89], [401, 107], [369, 78], [384, 57], [384, 85], [380, 100]]</t>
         </is>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A131" t="n">
+        <v>0</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>[[116, 357], [161, 338], [201, 302], [216, 260], [199, 235], [180, 261], [177, 229], [174, 267], [175, 279], [148, 259], [146, 233], [146, 277], [149, 280], [119, 261], [117, 237], [119, 279], [124, 286], [89, 264], [87, 248], [93, 278], [98, 286]]</t>
+          <t>[[387, 163], [440, 150], [475, 130], [496, 101], [492, 76], [461, 94], [473, 63], [466, 88], [458, 106], [438, 87], [450, 56], [442, 90], [434, 108], [413, 83], [426, 53], [421, 88], [414, 107], [383, 81], [398, 59], [398, 85], [395, 101]]</t>
         </is>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A132" t="n">
+        <v>0</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>[[127, 355], [172, 342], [214, 304], [230, 262], [215, 236], [193, 263], [194, 228], [188, 266], [187, 278], [163, 262], [162, 231], [160, 276], [162, 279], [134, 262], [133, 236], [134, 278], [138, 285], [105, 262], [104, 245], [108, 276], [113, 285]]</t>
+          <t>[[391, 165], [442, 152], [476, 130], [496, 103], [492, 78], [461, 93], [474, 64], [468, 90], [460, 109], [438, 87], [451, 58], [444, 92], [435, 111], [413, 84], [428, 55], [423, 92], [415, 111], [384, 82], [400, 60], [400, 87], [395, 104]]</t>
         </is>
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A133" t="n">
+        <v>0</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>[[146, 363], [187, 356], [230, 314], [246, 273], [233, 249], [211, 269], [212, 240], [209, 276], [211, 290], [181, 268], [181, 244], [181, 286], [182, 294], [153, 270], [152, 247], [155, 290], [157, 301], [122, 273], [123, 258], [128, 290], [130, 301]]</t>
+          <t>[[393, 168], [443, 155], [477, 133], [495, 105], [492, 80], [461, 95], [474, 68], [468, 95], [459, 114], [439, 89], [452, 61], [446, 96], [436, 114], [414, 86], [429, 60], [425, 96], [417, 114], [385, 86], [402, 64], [403, 91], [398, 106]]</t>
         </is>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A134" t="n">
+        <v>0</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>[[557, 343], [593, 318], [599, 287], [603, 264], [606, 244], [576, 260], [596, 242], [598, 266], [588, 282], [563, 257], [588, 237], [590, 270], [575, 285], [546, 254], [576, 236], [577, 271], [558, 284], [523, 254], [557, 241], [561, 265], [547, 277]]</t>
+          <t>[[394, 166], [446, 154], [478, 132], [497, 105], [494, 81], [462, 95], [476, 68], [470, 95], [460, 114], [440, 89], [454, 62], [447, 97], [437, 116], [416, 86], [431, 61], [426, 96], [418, 115], [388, 85], [404, 64], [405, 91], [400, 106]]</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A135" t="n">
+        <v>0</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>[[560, 350], [594, 322], [599, 291], [604, 269], [610, 250], [573, 261], [596, 245], [598, 270], [587, 284], [560, 258], [590, 241], [592, 274], [576, 289], [544, 257], [579, 241], [579, 276], [561, 289], [524, 259], [560, 247], [565, 272], [550, 283]]</t>
+          <t>[[393, 165], [445, 153], [478, 131], [496, 104], [493, 79], [462, 94], [476, 67], [470, 95], [460, 114], [440, 88], [454, 62], [447, 97], [437, 114], [416, 85], [432, 59], [427, 96], [418, 113], [388, 84], [405, 63], [406, 90], [400, 105]]</t>
         </is>
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A136" t="n">
+        <v>0</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>[[560, 350], [593, 322], [598, 291], [604, 269], [609, 248], [568, 260], [593, 244], [597, 269], [587, 284], [556, 258], [588, 240], [591, 274], [576, 289], [541, 256], [578, 242], [579, 277], [560, 290], [522, 258], [559, 247], [564, 272], [549, 284]]</t>
+          <t>[[397, 166], [445, 154], [477, 131], [495, 105], [493, 81], [462, 95], [476, 69], [472, 95], [462, 113], [441, 90], [456, 62], [450, 95], [439, 113], [417, 86], [433, 59], [430, 95], [420, 114], [389, 85], [407, 64], [409, 90], [402, 107]]</t>
         </is>
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A137" t="n">
+        <v>0</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>[[391, 432], [401, 388], [424, 355], [447, 344], [451, 359], [476, 383], [461, 370], [447, 372], [441, 378], [480, 408], [466, 392], [453, 393], [446, 400], [476, 429], [465, 414], [454, 413], [446, 418], [466, 446], [460, 434], [452, 432], [445, 435]]</t>
+          <t>[[325, 278], [288, 253], [267, 219], [266, 187], [278, 184], [299, 184], [308, 169], [307, 182], [303, 194], [328, 186], [330, 177], [327, 190], [325, 202], [352, 193], [348, 191], [344, 200], [342, 211], [372, 204], [365, 201], [361, 211], [358, 220]]</t>
         </is>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A138" t="n">
+        <v>0</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>[[388, 432], [399, 388], [423, 355], [447, 344], [451, 359], [475, 384], [461, 369], [446, 372], [440, 377], [479, 408], [465, 391], [452, 391], [445, 398], [474, 430], [463, 413], [453, 411], [445, 416], [464, 447], [459, 432], [450, 430], [443, 434]]</t>
+          <t>[[333, 286], [298, 257], [283, 224], [286, 195], [299, 187], [305, 192], [315, 179], [317, 192], [314, 203], [333, 193], [338, 187], [337, 199], [335, 211], [360, 201], [358, 201], [356, 212], [352, 223], [382, 214], [378, 214], [373, 225], [369, 234]]</t>
         </is>
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A139" t="n">
+        <v>0</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>[[394, 440], [404, 396], [429, 363], [453, 350], [454, 366], [478, 392], [463, 375], [449, 378], [444, 385], [482, 416], [467, 398], [454, 399], [448, 407], [476, 436], [465, 420], [455, 418], [449, 424], [466, 453], [461, 439], [453, 437], [446, 441]]</t>
+          <t>[[337, 285], [301, 256], [287, 225], [289, 197], [302, 186], [304, 197], [310, 180], [313, 190], [313, 204], [331, 196], [334, 183], [333, 193], [332, 206], [358, 201], [355, 194], [353, 204], [351, 216], [382, 212], [375, 207], [371, 216], [368, 226]]</t>
         </is>
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A140" t="n">
+        <v>0</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>[[393, 441], [403, 398], [427, 364], [451, 351], [454, 366], [479, 393], [462, 374], [448, 377], [442, 384], [483, 416], [467, 397], [453, 397], [446, 405], [477, 437], [465, 419], [455, 417], [448, 423], [466, 454], [461, 438], [452, 436], [446, 441]]</t>
+          <t>[[345, 281], [308, 256], [294, 222], [298, 193], [313, 187], [313, 197], [317, 178], [317, 191], [316, 205], [341, 196], [340, 181], [339, 193], [338, 205], [367, 201], [362, 191], [360, 202], [357, 214], [390, 211], [382, 203], [377, 212], [375, 222]]</t>
         </is>
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A141" t="n">
+        <v>0</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>[[391, 393], [416, 419], [446, 433], [474, 434], [484, 416], [463, 400], [486, 402], [461, 411], [450, 409], [458, 383], [479, 387], [450, 398], [442, 392], [451, 366], [473, 371], [445, 383], [435, 376], [441, 346], [460, 356], [441, 366], [431, 361]]</t>
+          <t>[[354, 280], [318, 257], [303, 219], [306, 187], [319, 186], [334, 194], [339, 175], [335, 187], [331, 201], [360, 197], [359, 183], [355, 194], [353, 206], [383, 205], [378, 194], [374, 204], [370, 216], [403, 216], [396, 205], [390, 214], [388, 224]]</t>
         </is>
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A142" t="n">
+        <v>0</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>[[392, 377], [417, 404], [446, 418], [473, 417], [482, 399], [457, 386], [480, 389], [459, 397], [447, 395], [453, 369], [475, 372], [448, 382], [438, 377], [447, 352], [469, 355], [443, 367], [432, 362], [437, 332], [457, 339], [440, 349], [430, 346]]</t>
+          <t>[[363, 282], [328, 255], [315, 219], [321, 189], [338, 188], [346, 197], [352, 177], [347, 189], [342, 203], [372, 201], [373, 186], [368, 196], [365, 209], [395, 211], [392, 199], [387, 208], [382, 220], [415, 225], [410, 211], [403, 219], [399, 229]]</t>
         </is>
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A143" t="n">
+        <v>0</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[[395, 378], [418, 408], [444, 422], [470, 422], [481, 405], [457, 390], [480, 392], [459, 400], [447, 399], [454, 373], [475, 375], [449, 385], [439, 380], [448, 356], [470, 360], [444, 370], [433, 364], [440, 335], [460, 346], [442, 355], [431, 350]]</t>
+          <t>[[289, 297], [333, 283], [364, 263], [378, 235], [368, 217], [345, 230], [352, 205], [347, 228], [343, 245], [324, 226], [330, 201], [327, 232], [324, 247], [302, 226], [309, 202], [308, 232], [306, 249], [277, 228], [286, 208], [289, 230], [288, 244]]</t>
         </is>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A144" t="n">
+        <v>0</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>[[394, 380], [418, 409], [444, 422], [470, 423], [482, 407], [458, 391], [481, 392], [459, 401], [447, 401], [454, 374], [476, 376], [449, 387], [439, 382], [447, 358], [470, 361], [444, 373], [433, 367], [439, 338], [459, 346], [443, 356], [432, 351]]</t>
+          <t>[[303, 303], [347, 289], [377, 268], [390, 240], [380, 221], [357, 234], [367, 210], [362, 236], [356, 252], [337, 231], [346, 207], [343, 239], [337, 253], [315, 230], [326, 207], [325, 239], [320, 254], [290, 232], [303, 213], [306, 236], [303, 249]]</t>
         </is>
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A145" t="n">
+        <v>1</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[[397, 380], [418, 408], [446, 423], [474, 423], [485, 406], [460, 392], [482, 393], [460, 402], [449, 401], [456, 375], [478, 377], [450, 388], [441, 382], [450, 358], [473, 362], [446, 373], [436, 367], [442, 338], [462, 346], [445, 356], [435, 352]]</t>
+          <t>[[155, 417], [205, 375], [233, 308], [221, 247], [183, 213], [227, 218], [234, 135], [230, 80], [226, 32], [176, 222], [190, 147], [201, 184], [209, 231], [126, 238], [137, 225], [148, 295], [155, 345], [80, 263], [96, 252], [111, 307], [118, 344]]</t>
         </is>
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A146" t="n">
+        <v>1</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>[[401, 383], [420, 412], [448, 428], [475, 427], [485, 412], [463, 397], [485, 399], [462, 407], [452, 405], [459, 379], [480, 383], [453, 392], [446, 386], [453, 362], [476, 367], [449, 377], [440, 371], [447, 341], [465, 351], [447, 360], [438, 355]]</t>
+          <t>[[133, 425], [176, 381], [197, 317], [180, 263], [140, 228], [185, 215], [180, 127], [167, 73], [158, 27], [134, 225], [140, 145], [136, 176], [135, 220], [84, 247], [86, 231], [101, 297], [114, 346], [41, 275], [45, 265], [65, 316], [80, 352]]</t>
         </is>
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A147" t="n">
+        <v>1</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>[[401, 385], [421, 414], [449, 429], [475, 430], [486, 414], [464, 399], [486, 400], [464, 409], [453, 409], [460, 381], [481, 385], [454, 395], [446, 389], [454, 364], [477, 369], [450, 380], [441, 374], [447, 344], [466, 355], [448, 363], [438, 357]]</t>
+          <t>[[140, 426], [183, 380], [206, 316], [189, 263], [148, 231], [190, 214], [185, 127], [172, 73], [164, 27], [138, 225], [144, 145], [143, 181], [144, 228], [89, 246], [94, 231], [108, 298], [121, 346], [46, 273], [52, 261], [71, 310], [85, 344]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>1</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>[[508, 463], [572, 444], [622, 399], [643, 364], [635, 338], [578, 294], [592, 218], [600, 167], [603, 125], [541, 285], [595, 230], [641, 236], [668, 253], [510, 290], [588, 305], [584, 359], [565, 388], [488, 310], [557, 343], [553, 382], [535, 399]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>1</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>[[488, 450], [554, 433], [615, 383], [650, 349], [666, 326], [578, 282], [594, 211], [603, 162], [607, 120], [544, 272], [595, 224], [644, 228], [676, 237], [513, 275], [582, 292], [579, 346], [562, 376], [489, 293], [551, 321], [548, 363], [533, 385]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>1</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>[[400, 409], [459, 382], [518, 324], [559, 280], [567, 237], [471, 226], [481, 152], [483, 104], [479, 65], [431, 221], [478, 163], [525, 184], [552, 216], [394, 229], [462, 235], [467, 296], [455, 333], [364, 250], [429, 271], [434, 317], [424, 345]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>1</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>[[392, 416], [455, 388], [514, 330], [554, 286], [563, 245], [464, 232], [473, 157], [476, 106], [474, 66], [425, 228], [471, 170], [520, 188], [548, 219], [390, 237], [458, 244], [464, 306], [453, 345], [362, 258], [425, 281], [428, 329], [416, 358]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>1</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>[[317, 451], [342, 436], [366, 406], [377, 378], [368, 364], [347, 355], [346, 310], [341, 285], [335, 264], [324, 355], [337, 320], [348, 338], [355, 359], [302, 361], [322, 361], [328, 394], [330, 418], [281, 371], [299, 378], [308, 404], [312, 421]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>1</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>[[317, 450], [343, 435], [365, 408], [377, 381], [373, 363], [348, 355], [348, 309], [343, 284], [337, 262], [325, 353], [340, 319], [352, 337], [359, 358], [303, 358], [325, 362], [331, 394], [332, 416], [283, 367], [303, 380], [311, 406], [315, 423]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>1</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>[[264, 340], [307, 321], [344, 270], [354, 218], [334, 180], [323, 209], [328, 145], [324, 106], [318, 72], [290, 209], [306, 150], [315, 167], [318, 190], [255, 217], [271, 191], [277, 244], [277, 282], [219, 230], [237, 218], [251, 258], [257, 287]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>1</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>[[267, 343], [310, 322], [347, 272], [360, 223], [342, 185], [326, 211], [330, 147], [326, 108], [322, 76], [293, 210], [310, 150], [318, 166], [322, 191], [259, 218], [277, 195], [281, 247], [281, 286], [223, 231], [241, 220], [254, 260], [260, 290]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>1</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>[[172, 358], [208, 335], [230, 292], [227, 247], [207, 215], [219, 253], [218, 208], [211, 178], [205, 150], [193, 253], [199, 214], [201, 210], [201, 210], [165, 260], [166, 239], [173, 275], [178, 304], [137, 271], [143, 262], [154, 292], [162, 315]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>1</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>[[159, 356], [191, 330], [210, 287], [210, 247], [191, 222], [198, 250], [197, 202], [191, 171], [185, 146], [173, 252], [179, 205], [181, 204], [180, 216], [146, 260], [148, 240], [155, 273], [161, 303], [119, 274], [124, 262], [134, 289], [142, 312]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>1</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>[[153, 360], [186, 332], [203, 288], [203, 249], [182, 228], [187, 252], [182, 202], [175, 172], [168, 146], [161, 256], [166, 212], [168, 209], [168, 216], [135, 266], [136, 245], [147, 278], [156, 308], [108, 282], [115, 268], [129, 294], [139, 316]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>1</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>[[165, 366], [197, 341], [216, 297], [217, 257], [195, 233], [201, 257], [199, 206], [193, 176], [188, 150], [175, 260], [182, 216], [188, 224], [191, 240], [149, 269], [153, 250], [164, 285], [171, 314], [122, 283], [130, 271], [144, 297], [153, 319]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>1</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>[[177, 368], [210, 346], [230, 304], [232, 264], [212, 239], [217, 261], [218, 213], [214, 182], [211, 156], [190, 264], [195, 218], [201, 225], [205, 242], [162, 272], [171, 255], [179, 291], [183, 320], [134, 285], [147, 277], [160, 305], [167, 327]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>1</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>[[537, 365], [570, 345], [593, 319], [613, 300], [631, 283], [554, 273], [559, 240], [561, 217], [562, 197], [540, 272], [579, 254], [605, 265], [619, 278], [530, 278], [575, 283], [574, 310], [564, 324], [526, 289], [564, 296], [564, 315], [555, 324]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>1</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>[[541, 367], [574, 350], [599, 326], [620, 308], [631, 295], [565, 277], [571, 244], [574, 221], [574, 202], [551, 276], [589, 260], [614, 272], [628, 286], [540, 281], [583, 292], [580, 316], [570, 329], [534, 291], [572, 303], [570, 319], [561, 327]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>1</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>[[536, 368], [570, 351], [595, 328], [616, 309], [631, 296], [562, 278], [569, 246], [573, 222], [574, 202], [547, 277], [586, 260], [611, 274], [624, 290], [537, 282], [580, 294], [578, 318], [567, 331], [532, 293], [570, 306], [567, 323], [557, 331]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>1</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>[[532, 368], [567, 351], [590, 327], [612, 310], [631, 294], [556, 278], [565, 245], [569, 221], [571, 201], [542, 276], [582, 260], [609, 274], [622, 289], [532, 282], [578, 294], [575, 319], [563, 331], [528, 294], [567, 306], [564, 324], [553, 332]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>1</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>[[533, 371], [568, 355], [592, 330], [612, 313], [630, 299], [558, 280], [566, 248], [570, 224], [572, 204], [544, 278], [584, 265], [610, 280], [623, 295], [534, 285], [578, 298], [575, 322], [563, 334], [530, 296], [567, 311], [565, 328], [554, 335]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>1</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>[[529, 368], [564, 350], [587, 326], [608, 309], [627, 294], [553, 276], [561, 244], [565, 220], [567, 199], [538, 275], [578, 260], [604, 275], [617, 291], [528, 282], [574, 294], [572, 319], [562, 331], [524, 295], [562, 308], [561, 325], [551, 332]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>1</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>[[200, 398], [240, 375], [270, 326], [268, 278], [238, 244], [264, 249], [274, 178], [273, 132], [273, 93], [225, 250], [239, 189], [240, 203], [239, 228], [185, 260], [195, 247], [201, 302], [202, 342], [148, 275], [162, 269], [170, 311], [171, 339]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>1</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>[[197, 373], [240, 347], [267, 299], [260, 249], [231, 213], [261, 223], [270, 153], [268, 107], [268, 67], [221, 225], [231, 161], [232, 186], [234, 220], [181, 237], [191, 224], [197, 279], [200, 316], [144, 252], [156, 240], [164, 282], [164, 310]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>1</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>[[188, 333], [229, 303], [250, 249], [241, 199], [215, 163], [243, 178], [250, 107], [248, 61], [247, 22], [203, 180], [211, 110], [207, 126], [204, 156], [164, 194], [173, 182], [179, 235], [182, 270], [127, 214], [140, 206], [149, 248], [153, 274]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>1</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>[[150, 349], [188, 315], [201, 261], [181, 213], [150, 184], [199, 189], [201, 118], [197, 71], [193, 33], [160, 194], [156, 123], [149, 145], [146, 180], [122, 211], [119, 195], [125, 239], [131, 272], [90, 235], [92, 216], [101, 248], [108, 274]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>1</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>[[90, 387], [122, 337], [120, 276], [76, 242], [39, 232], [114, 212], [104, 142], [93, 97], [88, 60], [75, 225], [58, 169], [39, 196], [35, 231], [42, 247], [23, 236], [33, 280], [51, 312], [19, 275], [4, 267], [17, 299], [36, 326]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>1</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>[[37, 392], [18, 350], [9, 298], [-1, 264], [-22, 233], [30, 222], [20, 157], [7, 116], [-6, 82], [36, 231], [25, 157], [8, 113], [-7, 77], [36, 261], [21, 199], [2, 180], [-12, 165], [33, 304], [16, 273], [-2, 266], [-16, 262]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>1</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>[[31, 395], [8, 340], [-10, 290], [-26, 255], [-46, 222], [2, 236], [-7, 174], [-18, 133], [-24, 100], [18, 254], [8, 185], [-4, 143], [-17, 107], [29, 286], [22, 225], [6, 185], [-8, 155], [33, 327], [14, 304], [-8, 288], [-30, 276]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>1</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>[[379, 372], [427, 350], [469, 308], [497, 274], [493, 251], [435, 228], [449, 168], [456, 130], [457, 98], [403, 225], [444, 185], [482, 204], [503, 231], [375, 232], [426, 246], [428, 289], [419, 316], [352, 248], [398, 264], [400, 296], [390, 317]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>1</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>[[426, 382], [477, 360], [521, 322], [553, 293], [569, 269], [487, 245], [502, 187], [510, 150], [513, 118], [459, 241], [508, 206], [545, 224], [566, 247], [434, 247], [488, 261], [483, 301], [469, 322], [415, 262], [461, 281], [458, 310], [445, 324]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>1</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>[[446, 385], [497, 365], [543, 325], [578, 297], [596, 273], [509, 250], [524, 195], [530, 159], [532, 129], [481, 246], [529, 210], [567, 229], [589, 252], [458, 252], [513, 267], [509, 306], [496, 327], [442, 267], [490, 287], [486, 316], [473, 329]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>1</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>[[435, 380], [482, 359], [523, 320], [555, 294], [570, 271], [491, 249], [507, 196], [516, 160], [520, 131], [465, 246], [509, 212], [545, 230], [566, 252], [441, 251], [491, 263], [487, 303], [473, 324], [420, 264], [465, 279], [462, 308], [449, 321]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>1</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>[[350, 371], [396, 351], [431, 315], [443, 283], [425, 264], [409, 240], [419, 184], [423, 147], [423, 118], [379, 238], [410, 193], [442, 209], [462, 232], [351, 244], [392, 256], [391, 296], [379, 316], [325, 258], [363, 271], [364, 299], [353, 312]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>1</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>[[269, 400], [311, 372], [339, 327], [344, 289], [331, 263], [308, 265], [308, 205], [304, 170], [297, 140], [276, 267], [295, 224], [311, 254], [316, 279], [248, 278], [279, 287], [287, 324], [282, 340], [223, 295], [256, 308], [264, 335], [260, 345]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>1</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>[[211, 435], [244, 404], [267, 361], [273, 325], [253, 308], [239, 293], [233, 233], [225, 197], [214, 167], [205, 298], [216, 256], [231, 286], [239, 315], [174, 312], [199, 317], [212, 360], [214, 383], [147, 330], [169, 339], [183, 368], [186, 382]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>1</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>[[209, 473], [243, 446], [265, 408], [267, 376], [246, 361], [246, 339], [243, 279], [237, 244], [232, 214], [214, 341], [223, 307], [233, 332], [241, 359], [183, 351], [200, 363], [210, 403], [215, 428], [156, 365], [173, 382], [183, 412], [188, 428]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>1</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>[[237, 504], [266, 479], [289, 446], [289, 420], [271, 403], [266, 375], [263, 320], [259, 287], [254, 258], [233, 378], [245, 347], [260, 379], [265, 404], [203, 390], [223, 400], [236, 437], [238, 452], [177, 408], [195, 422], [206, 447], [206, 454]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>1</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>[[242, 509], [271, 493], [297, 468], [305, 445], [289, 429], [278, 392], [275, 339], [272, 306], [267, 279], [245, 392], [261, 368], [275, 401], [279, 425], [216, 404], [237, 425], [248, 462], [249, 477], [190, 421], [209, 444], [222, 471], [222, 480]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>1</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>[[249, 489], [279, 470], [306, 438], [318, 410], [304, 395], [286, 371], [289, 320], [286, 288], [282, 261], [257, 370], [273, 339], [287, 366], [295, 393], [229, 377], [252, 390], [260, 427], [261, 450], [204, 390], [224, 408], [233, 434], [234, 447]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>1</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>[[235, 442], [269, 415], [291, 374], [292, 337], [270, 315], [273, 323], [274, 271], [271, 239], [269, 211], [244, 325], [254, 291], [265, 317], [273, 344], [216, 333], [234, 331], [242, 369], [245, 396], [190, 346], [207, 345], [216, 373], [220, 392]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>1</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>[[238, 377], [271, 353], [293, 315], [297, 279], [279, 255], [273, 266], [274, 215], [269, 185], [265, 158], [245, 268], [255, 230], [264, 233], [272, 241], [216, 275], [234, 270], [241, 309], [245, 339], [190, 287], [209, 286], [219, 316], [224, 338]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>1</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>[[278, 351], [314, 330], [344, 286], [342, 247], [324, 224], [322, 243], [323, 194], [320, 163], [317, 138], [295, 243], [304, 208], [318, 205], [329, 209], [269, 248], [286, 244], [292, 281], [295, 311], [243, 259], [264, 255], [272, 285], [274, 308]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>1</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>[[331, 324], [365, 307], [394, 272], [412, 240], [413, 211], [373, 221], [378, 173], [379, 145], [378, 121], [350, 219], [366, 185], [386, 184], [400, 189], [325, 222], [348, 221], [350, 258], [348, 286], [300, 230], [324, 231], [328, 259], [327, 280]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>1</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>[[370, 303], [406, 286], [435, 252], [451, 221], [460, 193], [409, 202], [417, 159], [420, 131], [422, 107], [389, 200], [412, 168], [436, 166], [453, 172], [367, 202], [398, 196], [397, 234], [392, 264], [346, 206], [376, 203], [379, 232], [376, 255]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>1</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>[[387, 282], [421, 268], [452, 236], [473, 205], [480, 176], [428, 188], [437, 147], [441, 120], [443, 98], [409, 185], [434, 153], [458, 151], [473, 158], [388, 185], [420, 175], [417, 213], [409, 243], [366, 188], [399, 183], [400, 212], [393, 236]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>1</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>[[377, 258], [412, 246], [442, 214], [463, 185], [471, 156], [422, 166], [431, 126], [434, 100], [436, 79], [403, 163], [426, 132], [447, 130], [462, 135], [380, 163], [409, 156], [406, 192], [400, 221], [357, 166], [386, 161], [389, 191], [384, 214]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>1</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>[[373, 256], [408, 241], [438, 208], [459, 179], [466, 150], [415, 165], [424, 125], [429, 99], [433, 78], [397, 162], [419, 132], [441, 128], [457, 132], [375, 162], [404, 151], [402, 187], [396, 217], [353, 164], [383, 157], [384, 186], [380, 210]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>1</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>[[274, 294], [311, 274], [344, 232], [353, 195], [335, 172], [323, 186], [330, 140], [332, 110], [332, 84], [297, 186], [311, 152], [327, 151], [338, 151], [270, 191], [293, 188], [295, 224], [291, 245], [242, 201], [267, 200], [272, 229], [269, 245]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>1</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>[[212, 301], [250, 274], [278, 232], [278, 193], [254, 170], [265, 189], [272, 138], [274, 107], [275, 81], [235, 189], [247, 152], [254, 167], [257, 184], [207, 195], [220, 192], [226, 229], [227, 254], [178, 206], [195, 206], [203, 235], [204, 253]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>1</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>[[157, 292], [189, 265], [209, 224], [211, 186], [190, 160], [203, 177], [211, 125], [213, 93], [213, 65], [175, 178], [183, 134], [191, 156], [195, 182], [146, 185], [156, 178], [161, 216], [161, 242], [118, 196], [131, 192], [139, 220], [140, 238]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>1</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>[[122, 292], [152, 267], [168, 229], [166, 193], [148, 167], [163, 177], [168, 125], [169, 91], [168, 61], [135, 179], [141, 133], [150, 150], [157, 175], [105, 189], [114, 174], [120, 213], [122, 241], [77, 202], [87, 187], [96, 216], [98, 237]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>1</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>[[96, 291], [123, 262], [133, 221], [125, 184], [103, 162], [133, 175], [135, 122], [133, 89], [132, 60], [104, 178], [106, 132], [106, 150], [109, 173], [76, 188], [77, 175], [83, 212], [88, 237], [50, 202], [53, 189], [62, 216], [66, 236]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>1</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>[[91, 293], [117, 266], [127, 229], [119, 193], [99, 168], [128, 175], [130, 126], [127, 94], [126, 65], [99, 180], [97, 136], [99, 155], [103, 179], [70, 191], [71, 179], [79, 216], [84, 243], [45, 205], [49, 196], [58, 223], [63, 244]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>1</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>[[204, 364], [240, 344], [270, 312], [277, 279], [257, 260], [255, 258], [263, 209], [267, 180], [269, 154], [228, 256], [243, 222], [254, 241], [260, 261], [201, 260], [220, 266], [224, 300], [223, 320], [176, 270], [195, 279], [201, 304], [200, 319]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>1</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>[[268, 381], [302, 368], [334, 338], [349, 312], [337, 295], [316, 280], [326, 232], [330, 202], [331, 178], [291, 275], [316, 245], [338, 263], [349, 284], [267, 279], [300, 293], [300, 324], [292, 339], [247, 289], [277, 306], [276, 329], [268, 339]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>1</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>[[339, 413], [377, 398], [408, 369], [429, 348], [443, 331], [386, 308], [399, 264], [407, 234], [412, 209], [364, 305], [400, 282], [426, 298], [442, 317], [345, 311], [387, 328], [383, 358], [372, 374], [330, 322], [365, 341], [364, 364], [355, 373]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>1</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>[[402, 425], [445, 407], [475, 378], [500, 361], [522, 347], [445, 316], [459, 275], [466, 246], [470, 222], [425, 314], [471, 297], [500, 315], [515, 333], [410, 323], [459, 340], [455, 368], [442, 381], [400, 338], [441, 356], [440, 376], [430, 385]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>1</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>[[440, 422], [484, 405], [513, 378], [539, 360], [562, 344], [481, 316], [496, 278], [504, 251], [508, 228], [464, 314], [512, 297], [543, 314], [560, 330], [453, 322], [505, 338], [499, 366], [485, 378], [450, 337], [493, 356], [489, 376], [477, 382]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>1</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>[[438, 423], [483, 406], [511, 378], [535, 359], [559, 345], [476, 316], [491, 278], [500, 251], [504, 227], [460, 315], [508, 297], [540, 315], [557, 333], [450, 324], [502, 339], [498, 368], [484, 380], [446, 339], [490, 358], [487, 377], [475, 383]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>1</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>[[392, 438], [429, 414], [454, 386], [474, 368], [489, 352], [424, 326], [431, 285], [436, 255], [438, 230], [402, 325], [440, 307], [469, 325], [483, 343], [385, 335], [431, 354], [430, 383], [417, 394], [374, 353], [415, 374], [414, 394], [401, 399]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>1</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>[[345, 441], [383, 420], [409, 391], [427, 368], [439, 349], [378, 330], [384, 285], [387, 256], [389, 232], [357, 330], [391, 307], [420, 322], [438, 341], [339, 340], [384, 354], [385, 384], [377, 399], [327, 356], [367, 372], [369, 393], [361, 403]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>1</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>[[313, 444], [345, 423], [371, 395], [387, 372], [385, 356], [344, 338], [350, 292], [352, 263], [350, 238], [320, 337], [346, 308], [372, 326], [386, 345], [300, 345], [338, 360], [340, 392], [331, 406], [283, 359], [317, 376], [319, 398], [311, 406]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>1</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>[[276, 440], [307, 421], [332, 394], [349, 374], [356, 359], [311, 336], [319, 289], [323, 260], [323, 236], [288, 334], [314, 306], [337, 327], [349, 348], [267, 340], [301, 357], [306, 389], [300, 404], [249, 352], [278, 372], [282, 395], [275, 403]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>1</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>[[227, 420], [258, 403], [285, 373], [295, 347], [281, 333], [268, 317], [275, 272], [278, 245], [277, 221], [243, 316], [260, 287], [275, 308], [281, 330], [219, 322], [244, 333], [248, 364], [243, 380], [198, 334], [222, 345], [226, 368], [220, 378]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>1</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>[[181, 409], [210, 389], [234, 359], [240, 333], [223, 321], [221, 306], [225, 260], [226, 233], [226, 210], [194, 306], [206, 277], [215, 300], [220, 320], [169, 312], [187, 323], [193, 355], [194, 370], [147, 322], [164, 336], [171, 359], [173, 369]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>1</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>[[169, 394], [198, 375], [220, 346], [226, 320], [211, 303], [210, 290], [214, 245], [213, 216], [212, 191], [183, 288], [194, 257], [200, 278], [205, 302], [156, 293], [170, 306], [176, 339], [179, 361], [132, 303], [145, 317], [153, 342], [157, 357]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>1</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>[[163, 374], [194, 352], [216, 319], [218, 286], [197, 267], [201, 269], [207, 222], [206, 194], [205, 168], [175, 268], [185, 236], [193, 256], [199, 278], [148, 275], [164, 279], [171, 314], [173, 337], [124, 286], [139, 293], [147, 318], [149, 332]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>1</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>[[134, 328], [163, 304], [179, 267], [177, 232], [155, 212], [163, 223], [163, 173], [159, 143], [155, 116], [136, 225], [142, 189], [150, 205], [157, 224], [110, 233], [121, 231], [131, 266], [137, 290], [85, 246], [98, 246], [110, 272], [116, 289]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>1</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>[[131, 307], [160, 283], [173, 248], [170, 213], [152, 187], [158, 197], [156, 148], [152, 118], [149, 91], [130, 201], [137, 159], [143, 179], [147, 203], [102, 210], [114, 202], [124, 239], [129, 265], [77, 221], [90, 217], [102, 247], [107, 267]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>1</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>[[192, 302], [225, 274], [247, 233], [244, 196], [221, 176], [225, 191], [227, 143], [224, 113], [221, 87], [198, 194], [207, 158], [218, 161], [225, 169], [172, 201], [189, 196], [197, 232], [200, 259], [146, 214], [166, 211], [177, 238], [180, 259]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>1</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>[[226, 296], [262, 272], [289, 233], [296, 198], [278, 175], [262, 186], [265, 138], [264, 109], [262, 84], [235, 187], [245, 152], [261, 157], [274, 168], [208, 194], [231, 193], [239, 228], [241, 254], [183, 206], [208, 206], [219, 235], [224, 256]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>1</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>[[285, 289], [318, 269], [348, 237], [365, 210], [361, 189], [321, 185], [329, 137], [333, 108], [334, 84], [298, 184], [319, 149], [341, 156], [356, 172], [275, 188], [305, 189], [308, 226], [306, 253], [253, 197], [281, 200], [287, 229], [287, 251]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>1</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>[[348, 307], [382, 290], [411, 259], [428, 235], [437, 212], [389, 207], [401, 163], [409, 135], [413, 112], [368, 203], [399, 175], [424, 184], [438, 198], [349, 205], [383, 211], [380, 245], [370, 265], [329, 213], [362, 220], [362, 245], [355, 260]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>1</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>[[403, 342], [438, 329], [469, 300], [494, 279], [511, 260], [448, 242], [462, 201], [471, 173], [476, 150], [429, 237], [468, 212], [495, 226], [510, 244], [411, 238], [451, 249], [444, 280], [430, 297], [396, 245], [432, 260], [428, 284], [416, 295]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>1</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>[[378, 332], [415, 317], [447, 287], [467, 264], [482, 246], [429, 232], [443, 194], [451, 168], [455, 145], [410, 229], [441, 202], [468, 217], [484, 235], [392, 231], [431, 240], [425, 272], [413, 288], [376, 238], [411, 250], [408, 273], [397, 283]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>1</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>[[317, 317], [351, 300], [381, 269], [400, 243], [406, 219], [357, 217], [369, 175], [376, 147], [380, 124], [337, 215], [363, 183], [387, 192], [401, 207], [316, 219], [350, 224], [348, 258], [339, 277], [296, 227], [328, 233], [329, 260], [321, 274]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>1</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>[[289, 326], [320, 310], [349, 280], [367, 253], [367, 229], [322, 226], [334, 181], [340, 153], [343, 128], [300, 224], [326, 192], [351, 202], [365, 218], [279, 228], [313, 231], [312, 266], [304, 288], [259, 238], [291, 243], [294, 270], [288, 287]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>1</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>[[272, 343], [303, 328], [332, 297], [351, 272], [351, 253], [310, 242], [322, 198], [327, 169], [330, 144], [287, 240], [310, 209], [333, 221], [347, 240], [265, 244], [296, 250], [296, 285], [290, 308], [244, 253], [274, 262], [276, 289], [272, 306]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>1</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>[[267, 357], [298, 341], [326, 313], [343, 287], [338, 269], [305, 258], [317, 214], [322, 186], [325, 162], [282, 256], [304, 227], [325, 240], [339, 258], [260, 260], [289, 267], [290, 303], [285, 327], [238, 269], [267, 280], [269, 306], [264, 323]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>1</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>[[261, 359], [293, 343], [322, 313], [339, 286], [335, 268], [300, 256], [312, 214], [317, 186], [320, 162], [277, 255], [298, 227], [319, 240], [333, 259], [254, 259], [286, 265], [288, 301], [284, 326], [233, 269], [263, 279], [267, 306], [264, 324]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>1</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>[[256, 387], [287, 371], [314, 340], [330, 315], [327, 297], [296, 286], [307, 241], [311, 211], [314, 186], [273, 284], [296, 253], [316, 267], [328, 285], [251, 287], [280, 292], [281, 327], [276, 350], [230, 296], [257, 304], [260, 330], [256, 347]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>1</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>[[255, 424], [284, 410], [310, 383], [324, 362], [322, 346], [293, 326], [303, 279], [307, 251], [310, 228], [269, 324], [290, 297], [310, 313], [321, 332], [246, 329], [274, 341], [278, 370], [273, 387], [226, 340], [252, 355], [255, 377], [249, 389]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>1</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>[[158, 470], [181, 448], [195, 418], [192, 397], [173, 387], [174, 367], [172, 325], [169, 299], [164, 278], [149, 374], [154, 349], [165, 374], [171, 393], [127, 387], [138, 388], [150, 415], [154, 428], [107, 403], [117, 405], [129, 424], [133, 432]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>1</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>[[130, 457], [151, 432], [162, 404], [158, 380], [139, 368], [147, 352], [144, 310], [139, 282], [134, 258], [121, 356], [123, 328], [133, 358], [139, 382], [98, 367], [104, 371], [116, 402], [122, 417], [77, 382], [84, 389], [95, 410], [101, 419]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>1</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>[[110, 446], [131, 421], [141, 394], [137, 372], [118, 360], [129, 343], [127, 298], [123, 271], [118, 247], [104, 346], [105, 313], [110, 342], [115, 369], [80, 355], [84, 360], [94, 391], [102, 409], [59, 367], [64, 374], [74, 396], [81, 408]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>1</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>[[101, 421], [123, 401], [134, 375], [130, 349], [116, 330], [127, 321], [126, 275], [122, 246], [119, 221], [102, 324], [104, 293], [106, 325], [109, 352], [79, 332], [81, 330], [88, 360], [93, 379], [58, 342], [60, 340], [69, 361], [74, 375]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>1</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>[[129, 389], [155, 370], [170, 345], [171, 319], [159, 300], [164, 292], [165, 247], [165, 220], [163, 197], [139, 292], [142, 269], [146, 303], [148, 331], [115, 298], [118, 303], [125, 333], [128, 352], [94, 307], [98, 310], [106, 331], [109, 344]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>1</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>[[177, 367], [206, 347], [225, 315], [228, 285], [212, 267], [212, 269], [217, 226], [219, 199], [219, 176], [187, 269], [197, 237], [206, 249], [212, 267], [163, 273], [179, 278], [185, 309], [187, 331], [141, 283], [157, 290], [165, 314], [169, 331]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>1</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>[[363, 343], [395, 326], [421, 298], [437, 277], [448, 258], [399, 248], [410, 210], [416, 185], [420, 164], [381, 246], [411, 220], [436, 228], [450, 239], [363, 249], [400, 252], [396, 283], [386, 300], [348, 257], [381, 262], [380, 284], [372, 295]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>1</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>[[426, 343], [456, 327], [481, 296], [502, 275], [513, 254], [453, 248], [462, 209], [467, 184], [470, 164], [437, 245], [468, 219], [494, 227], [510, 241], [420, 248], [458, 250], [455, 279], [442, 296], [406, 254], [442, 259], [442, 281], [431, 292]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>1</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>[[258, 434], [236, 387], [243, 348], [268, 326], [289, 320], [264, 326], [267, 276], [271, 248], [274, 225], [294, 336], [296, 296], [284, 306], [274, 321], [315, 353], [308, 330], [298, 338], [292, 350], [330, 370], [322, 350], [314, 358], [310, 368]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>1</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>[[257, 384], [234, 338], [243, 298], [264, 278], [284, 276], [261, 269], [264, 222], [267, 198], [270, 179], [290, 276], [290, 245], [281, 258], [272, 273], [314, 292], [303, 278], [295, 289], [288, 302], [331, 309], [320, 297], [313, 306], [309, 317]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>1</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>[[259, 385], [235, 338], [243, 296], [264, 272], [283, 266], [264, 267], [267, 217], [270, 191], [272, 170], [294, 274], [293, 240], [281, 253], [272, 269], [319, 291], [307, 273], [296, 284], [290, 298], [336, 308], [325, 292], [317, 302], [313, 315]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>1</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>[[258, 388], [235, 339], [243, 297], [264, 273], [284, 268], [263, 267], [267, 216], [270, 190], [273, 168], [294, 275], [293, 239], [281, 252], [271, 268], [319, 292], [306, 271], [296, 282], [289, 297], [337, 310], [324, 292], [316, 301], [312, 314]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>1</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>[[252, 395], [228, 343], [238, 299], [260, 274], [281, 269], [259, 271], [265, 215], [269, 187], [272, 163], [292, 279], [293, 239], [279, 253], [268, 270], [317, 297], [306, 275], [294, 286], [287, 302], [335, 316], [324, 297], [315, 307], [310, 321]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>1</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>[[343, 334], [313, 282], [320, 234], [344, 211], [365, 208], [352, 195], [355, 150], [356, 123], [358, 103], [387, 204], [385, 189], [373, 205], [368, 220], [412, 227], [403, 218], [392, 230], [387, 244], [430, 249], [424, 239], [416, 249], [411, 264]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>1</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>[[369, 253], [341, 212], [346, 172], [366, 152], [380, 148], [378, 129], [379, 95], [378, 77], [382, 64], [411, 135], [407, 138], [397, 153], [393, 166], [435, 156], [424, 161], [413, 173], [408, 184], [450, 177], [440, 180], [431, 188], [425, 198]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>1</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>[[364, 259], [339, 218], [345, 179], [369, 164], [386, 163], [376, 138], [377, 105], [379, 86], [383, 73], [409, 144], [406, 148], [399, 163], [396, 174], [432, 164], [423, 171], [415, 182], [409, 191], [447, 186], [440, 190], [432, 198], [426, 206]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>1</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>[[302, 278], [282, 233], [295, 194], [315, 174], [333, 170], [316, 155], [323, 121], [327, 101], [332, 87], [347, 160], [348, 158], [340, 172], [335, 183], [371, 179], [365, 180], [355, 190], [349, 201], [388, 199], [382, 198], [374, 206], [368, 216]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>1</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>[[235, 298], [215, 252], [229, 214], [251, 191], [270, 184], [248, 172], [260, 132], [266, 111], [272, 96], [278, 179], [286, 162], [277, 173], [269, 186], [302, 197], [300, 189], [289, 200], [281, 211], [320, 217], [315, 209], [306, 217], [298, 227]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>1</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>[[186, 312], [171, 262], [186, 224], [209, 204], [229, 199], [202, 185], [215, 145], [223, 124], [229, 108], [230, 193], [244, 173], [239, 185], [230, 198], [253, 211], [257, 202], [249, 214], [239, 225], [271, 231], [271, 224], [263, 233], [253, 242]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>1</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>[[135, 338], [117, 288], [130, 251], [151, 229], [172, 223], [143, 214], [157, 168], [164, 146], [170, 128], [169, 219], [189, 196], [185, 211], [176, 225], [193, 237], [200, 227], [192, 241], [184, 253], [212, 256], [212, 250], [205, 261], [197, 272]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>1</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>[[159, 515], [140, 474], [147, 436], [169, 412], [190, 405], [156, 410], [161, 356], [165, 325], [168, 301], [184, 419], [196, 372], [188, 385], [180, 402], [208, 435], [214, 401], [205, 412], [198, 425], [228, 453], [229, 424], [220, 432], [216, 444]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>1</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>[[180, 502], [163, 458], [171, 421], [191, 399], [211, 391], [182, 399], [189, 349], [193, 320], [197, 296], [210, 408], [220, 366], [212, 379], [204, 395], [233, 424], [235, 399], [227, 409], [220, 421], [251, 442], [248, 420], [240, 429], [236, 440]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>1</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>[[247, 475], [229, 428], [237, 390], [259, 369], [280, 365], [253, 367], [258, 319], [263, 292], [266, 270], [282, 377], [286, 339], [278, 350], [270, 366], [305, 394], [300, 375], [292, 385], [285, 397], [323, 412], [316, 395], [309, 404], [304, 415]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>1</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>[[288, 472], [267, 426], [271, 385], [291, 363], [310, 359], [300, 360], [303, 313], [306, 287], [307, 266], [329, 372], [327, 335], [315, 345], [307, 359], [350, 388], [338, 367], [328, 375], [321, 387], [363, 405], [352, 386], [344, 393], [340, 403]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>1</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>[[330, 469], [309, 424], [312, 379], [334, 361], [357, 368], [346, 360], [348, 313], [350, 288], [352, 269], [375, 371], [372, 339], [360, 351], [352, 366], [395, 389], [382, 370], [372, 379], [366, 390], [407, 406], [398, 389], [390, 396], [385, 406]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>1</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>[[375, 455], [356, 409], [355, 363], [376, 344], [397, 351], [396, 345], [393, 301], [393, 277], [394, 258], [425, 357], [416, 328], [401, 339], [393, 353], [443, 375], [427, 356], [415, 364], [408, 377], [453, 392], [441, 375], [432, 382], [428, 394]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>1</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>[[408, 435], [383, 392], [379, 349], [392, 327], [407, 330], [424, 326], [421, 281], [420, 258], [421, 240], [452, 338], [436, 316], [420, 328], [416, 341], [468, 356], [450, 338], [437, 345], [432, 357], [477, 372], [463, 356], [453, 362], [448, 374]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>1</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>[[438, 434], [416, 392], [411, 348], [422, 328], [437, 335], [461, 330], [454, 288], [450, 265], [452, 247], [487, 343], [467, 322], [452, 334], [448, 346], [500, 360], [481, 342], [468, 349], [464, 360], [507, 376], [493, 359], [483, 364], [479, 376]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>1</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>[[463, 414], [439, 377], [429, 335], [433, 315], [444, 322], [479, 313], [472, 274], [468, 253], [468, 235], [504, 325], [482, 308], [468, 320], [466, 331], [517, 342], [498, 326], [485, 334], [482, 345], [525, 358], [510, 344], [500, 350], [497, 362]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>1</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>[[492, 408], [469, 373], [460, 334], [459, 317], [462, 322], [514, 315], [501, 277], [495, 257], [495, 240], [536, 328], [512, 310], [496, 320], [493, 331], [546, 345], [526, 329], [511, 335], [508, 344], [550, 360], [535, 346], [524, 351], [521, 361]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>1</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>[[501, 382], [478, 348], [467, 311], [464, 296], [466, 301], [519, 289], [507, 255], [501, 235], [501, 219], [542, 301], [519, 286], [503, 297], [501, 308], [554, 318], [534, 304], [521, 310], [518, 319], [558, 334], [543, 321], [534, 325], [530, 335]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>1</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>[[499, 346], [471, 315], [460, 279], [456, 267], [455, 271], [510, 252], [497, 221], [489, 203], [489, 188], [534, 264], [513, 255], [497, 266], [494, 277], [546, 282], [527, 273], [514, 279], [510, 287], [553, 298], [537, 289], [527, 293], [524, 302]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>1</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>[[487, 280], [458, 248], [444, 214], [441, 201], [442, 204], [487, 177], [474, 146], [466, 128], [465, 113], [513, 184], [494, 178], [482, 192], [480, 203], [530, 202], [511, 195], [501, 203], [498, 213], [539, 218], [524, 211], [516, 217], [513, 227]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>1</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>[[490, 254], [460, 224], [444, 187], [440, 171], [446, 174], [491, 149], [476, 115], [468, 96], [467, 80], [518, 158], [495, 148], [482, 162], [481, 175], [533, 175], [514, 165], [502, 174], [499, 185], [542, 191], [526, 181], [517, 188], [515, 199]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>1</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>[[151, 288], [127, 240], [138, 203], [153, 179], [173, 171], [149, 162], [157, 116], [160, 93], [163, 74], [176, 165], [188, 142], [183, 158], [176, 173], [201, 181], [203, 170], [196, 184], [189, 197], [222, 198], [219, 190], [212, 201], [206, 213]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>1</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>[[176, 436], [211, 402], [224, 346], [207, 296], [175, 262], [221, 269], [218, 200], [210, 157], [203, 119], [182, 276], [182, 211], [180, 234], [182, 265], [144, 292], [148, 277], [159, 327], [167, 361], [112, 313], [120, 300], [133, 339], [143, 366]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>1</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>[[167, 459], [201, 426], [215, 377], [195, 338], [161, 313], [202, 283], [195, 212], [184, 168], [175, 131], [162, 294], [156, 241], [148, 275], [147, 313], [125, 312], [122, 313], [135, 364], [149, 399], [96, 333], [93, 329], [106, 364], [121, 390]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>1</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>[[167, 455], [200, 418], [214, 371], [193, 334], [159, 309], [199, 278], [190, 207], [179, 163], [169, 126], [158, 289], [153, 236], [146, 275], [146, 315], [121, 309], [119, 308], [133, 360], [147, 394], [92, 333], [90, 327], [106, 364], [123, 388]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>1</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>[[170, 452], [205, 416], [220, 368], [199, 331], [165, 307], [204, 275], [194, 206], [183, 162], [175, 125], [164, 286], [159, 233], [152, 274], [155, 314], [129, 305], [126, 303], [137, 354], [152, 387], [101, 327], [94, 319], [107, 353], [124, 377]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>1</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>[[164, 454], [198, 417], [209, 365], [173, 332], [134, 318], [188, 278], [178, 206], [169, 162], [160, 126], [148, 291], [141, 242], [141, 285], [147, 325], [113, 313], [109, 306], [123, 354], [136, 383], [86, 339], [79, 326], [93, 356], [110, 378]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>1</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>[[131, 455], [163, 415], [164, 364], [121, 339], [79, 322], [143, 274], [126, 205], [111, 162], [99, 126], [102, 291], [79, 250], [78, 293], [86, 331], [68, 318], [52, 317], [74, 366], [97, 393], [44, 347], [29, 343], [49, 376], [73, 394]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>1</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>[[192, 450], [226, 412], [243, 364], [223, 327], [187, 310], [223, 278], [211, 203], [201, 159], [193, 122], [184, 287], [179, 235], [184, 278], [191, 318], [149, 304], [149, 304], [159, 350], [170, 378], [118, 323], [116, 319], [127, 349], [136, 368]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>1</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>[[351, 425], [402, 402], [445, 358], [456, 318], [426, 296], [425, 268], [426, 199], [422, 156], [416, 120], [382, 265], [400, 227], [423, 259], [437, 287], [344, 278], [371, 300], [380, 338], [379, 351], [311, 301], [335, 324], [344, 349], [342, 352]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>1</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>[[454, 436], [511, 418], [559, 383], [592, 357], [597, 337], [526, 288], [538, 224], [542, 183], [542, 149], [489, 282], [536, 247], [568, 282], [582, 318], [457, 292], [513, 323], [513, 367], [501, 387], [433, 312], [479, 348], [479, 377], [465, 384]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>1</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>[[282, 372], [321, 338], [344, 292], [340, 252], [326, 225], [320, 232], [321, 164], [319, 126], [314, 95], [286, 234], [303, 184], [320, 215], [326, 245], [256, 245], [286, 252], [302, 293], [305, 315], [229, 262], [256, 266], [271, 290], [273, 302]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>1</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>[[180, 371], [214, 326], [224, 273], [206, 234], [175, 219], [208, 232], [205, 168], [202, 128], [199, 95], [177, 241], [181, 192], [189, 222], [194, 255], [147, 255], [153, 241], [166, 278], [173, 304], [120, 273], [128, 257], [142, 282], [147, 302]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>1</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>[[102, 348], [128, 306], [129, 257], [101, 219], [67, 203], [119, 204], [114, 145], [105, 108], [99, 76], [86, 215], [73, 159], [72, 183], [77, 213], [56, 235], [51, 222], [67, 260], [81, 288], [31, 261], [27, 243], [44, 269], [60, 291]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>1</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>[[52, 335], [76, 299], [80, 250], [53, 211], [20, 187], [74, 185], [65, 131], [54, 96], [45, 66], [42, 194], [18, 152], [7, 184], [9, 221], [11, 211], [-9, 197], [0, 240], [17, 275], [-12, 232], [-28, 221], [-14, 255], [4, 284]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>1</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>[[47, 306], [67, 271], [64, 227], [38, 193], [5, 163], [61, 165], [50, 113], [40, 78], [33, 49], [31, 179], [12, 140], [-3, 146], [-12, 161], [4, 199], [-11, 177], [-7, 211], [2, 240], [-17, 218], [-32, 208], [-24, 234], [-9, 255]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>1</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>[[142, 308], [171, 275], [178, 228], [163, 186], [135, 164], [167, 175], [165, 118], [160, 82], [155, 51], [138, 183], [133, 132], [140, 145], [148, 168], [111, 199], [108, 181], [123, 214], [134, 241], [85, 219], [85, 203], [102, 228], [113, 248]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>1</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>[[194, 321], [228, 286], [241, 239], [232, 195], [203, 175], [227, 193], [227, 136], [225, 99], [223, 68], [198, 198], [199, 160], [208, 189], [216, 222], [169, 209], [175, 198], [186, 235], [193, 265], [143, 225], [150, 215], [163, 242], [170, 265]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>1</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>[[476, 289], [508, 290], [544, 262], [570, 239], [581, 209], [516, 202], [525, 155], [533, 122], [534, 95], [490, 199], [526, 166], [557, 184], [570, 204], [468, 206], [514, 209], [513, 248], [499, 266], [451, 220], [494, 232], [494, 260], [481, 272]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>1</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>[[481, 312], [521, 293], [555, 257], [581, 228], [595, 201], [522, 196], [534, 145], [542, 113], [544, 86], [497, 194], [534, 155], [565, 169], [581, 191], [475, 199], [519, 206], [518, 243], [507, 265], [457, 211], [499, 220], [500, 248], [490, 264]]</t>
         </is>
       </c>
     </row>

</xml_diff>